<commit_message>
Update rules and characters powers
</commit_message>
<xml_diff>
--- a/src/resources/horde_cards.xlsx
+++ b/src/resources/horde_cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsaban/git/perso/windwalkers-cardgame/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA182F7-47E1-504B-B18C-C04AA5C89BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCC90BB-55D2-BB44-878B-A1C4467B6CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{2F94C834-2D3B-4040-A9EF-5D9A64AD9988}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -248,24 +248,12 @@
     <t>Arabine sait danser; elle danse si bien que le vent lui meme s'arrete pour la voir bouger.</t>
   </si>
   <si>
-    <t>τ:Placez sur la face souhaitee chaque d6 avec la meme valeur que la force du vent</t>
-  </si>
-  <si>
     <t>Nouchka.png</t>
   </si>
   <si>
-    <t>Alwine Böhnisch</t>
-  </si>
-  <si>
     <t>ranger</t>
   </si>
   <si>
-    <t>Alwine a un sens de l'orientation hors du commun qui se precise en zones boisees.</t>
-  </si>
-  <si>
-    <t>τ:Les d6 colores sont incolores</t>
-  </si>
-  <si>
     <t>Iphaine.png</t>
   </si>
   <si>
@@ -431,9 +419,6 @@
     <t xml:space="preserve">aeromaitresse </t>
   </si>
   <si>
-    <t xml:space="preserve">Hannicia </t>
-  </si>
-  <si>
     <t xml:space="preserve">airpailleuse </t>
   </si>
   <si>
@@ -443,9 +428,6 @@
     <t xml:space="preserve">peintre et poetesse </t>
   </si>
   <si>
-    <t xml:space="preserve">τ:Definissez une valeur de d6. Gagnez autant de moral que de d6 colores identiques a ce d6 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Oshora </t>
   </si>
   <si>
@@ -557,24 +539,15 @@
     <t xml:space="preserve">Quand Rochelle s'isole le vent se calme et le sang coule et personne ne pose de question. </t>
   </si>
   <si>
-    <t xml:space="preserve">Saskia Böhnisch </t>
-  </si>
-  <si>
     <t xml:space="preserve">archere </t>
   </si>
   <si>
-    <t xml:space="preserve">τ:Sur un terrain ayant exactement 2 d6 colores gagnez 1 point de moral </t>
-  </si>
-  <si>
     <t xml:space="preserve">Bertram Haring </t>
   </si>
   <si>
     <t xml:space="preserve">τ:Baissez la force du vent de 1 </t>
   </si>
   <si>
-    <t xml:space="preserve">Oliver Haucksson </t>
-  </si>
-  <si>
     <t xml:space="preserve">feuleur et acrobate </t>
   </si>
   <si>
@@ -584,9 +557,6 @@
     <t xml:space="preserve">sourciere </t>
   </si>
   <si>
-    <t xml:space="preserve">τ:Ne perdez pas de moral en utilsant vos allies </t>
-  </si>
-  <si>
     <t xml:space="preserve">Laenar </t>
   </si>
   <si>
@@ -746,9 +716,6 @@
     <t xml:space="preserve">Ed a une compréhension du vent qui dépasse beaucoup celle du commun des mortels. Il a cet instinct que d'autres (Kunigunde en tête) lui envient. </t>
   </si>
   <si>
-    <t xml:space="preserve">Les cerfs-volants d'Hannicia sont un ravissement qui suivent des courants bien spécifiques. Chacun nécessite un réglage particulier pour délester le groupe. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Josmina se définie comme une femme de la terre et une esthète. Ses œuvres ont aussi belles que manichéennes. Si le beau existe il doit être minéral ou végétal. </t>
   </si>
   <si>
@@ -1010,9 +977,6 @@
     <t>Thutmus est un excellent negociant qui trouve toujours la perle rare dont vous aurez besoin.</t>
   </si>
   <si>
-    <t>τ:Piochez une carte consommable</t>
-  </si>
-  <si>
     <t>Thutmus.png</t>
   </si>
   <si>
@@ -1091,9 +1055,6 @@
     <t>τ:Abandonnez-le et lancez 1d6 noir de contre supplementaire; 2d6 noirs si vous avez un autre Torantor</t>
   </si>
   <si>
-    <t xml:space="preserve">τ:Sur un terrain ayant exactement 3 d6 colores gagnez 2 point de moral </t>
-  </si>
-  <si>
     <t xml:space="preserve">Vera démonte et remonte les gens comme on le ferait avec un pantin. Ses talents de rebouteuse remettent l'aplomb les Hordiers les plus mal en point. </t>
   </si>
   <si>
@@ -1448,12 +1409,6 @@
     <t>τ:Faites -1 ou +1 sur chaque d6 du vent colore</t>
   </si>
   <si>
-    <t>τ:Lancez autant de d6 supplementaires que de vents de meme force sur le plateau. Ce vent ne compte pas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">τ:Gagnez 1 point de moral lorsque le vent fait un 1 </t>
-  </si>
-  <si>
     <t xml:space="preserve">τ:Ignorez 1 d6 du vent </t>
   </si>
   <si>
@@ -1493,16 +1448,61 @@
     <t>τ:Abandonnez un hordier de TRAINE. N'appliquez pas son pouvoir. Remplacez le par votre Faucon.</t>
   </si>
   <si>
-    <t>τ:Lancez 1d6 de moins et marquez 1 point de plus par tuile passee ce tour-ci. Cette tuile comptera egalement.</t>
-  </si>
-  <si>
     <t>τ:Retournez au plus autant de d6 du vent que de Hordiers de TRAINE</t>
   </si>
   <si>
-    <t>τ:Faites +/-1 sur vos d6. Triplez ce bonus si vous avez un Faucon</t>
-  </si>
-  <si>
     <t>τ:Abandonnez-la et recrutez un Hordier dans un village. Le hordier remplace est abandonne.</t>
+  </si>
+  <si>
+    <t>τ:Marquez 1 point de plus par tuile passee ce tour-ci. Cette tuile comptera egalement.</t>
+  </si>
+  <si>
+    <t>τ: Gagnez autant de moral que de d6 colores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anika </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les cerfs-volants d'Anika sont un ravissement qui suivent des courants bien spécifiques. Chacun nécessite un réglage particulier pour délester le groupe. </t>
+  </si>
+  <si>
+    <t>τ:Revelez un vent adjacent. Lancez autant de d6 supplementaires que de vents de meme force sur le plateau. Ce vent ne compte pas.</t>
+  </si>
+  <si>
+    <t>Eyline Bisch</t>
+  </si>
+  <si>
+    <t>Eyline a un sens de l'orientation hors du commun qui se precise en zones boisees.</t>
+  </si>
+  <si>
+    <t>τ:Gagnez autant de moral que de d6 noirs</t>
+  </si>
+  <si>
+    <t>τ:Ignorez les d6 du vent inferieurs a votre d6 le plus faible.</t>
+  </si>
+  <si>
+    <t>τ:Faites +/-1 sur vos d6 par oiseleur. Appliquez ce bonus 2 fois si vous avez un Faucon</t>
+  </si>
+  <si>
+    <t>τ:Gagnez 1d6 par penalite de moral.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oliver Hawksson </t>
+  </si>
+  <si>
+    <t xml:space="preserve">τ:Sur un terrain ayant exactement 3 d6 colores gagnez 3 point de moral </t>
+  </si>
+  <si>
+    <t>τ:Ne perdez pas de moral en utilsant un allie ou gagnez un point de moral.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saskia Bisch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">τ:Sur un terrain ayant exactement 2 d6 colores gagnez 2 point de moral </t>
+  </si>
+  <si>
+    <t>τ:Piochez une carte consommable ou marquez un point.</t>
   </si>
 </sst>
 </file>
@@ -3070,7 +3070,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4C07DF30-360B-9D4E-92AA-D9ACB16D7C47}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4C07DF30-360B-9D4E-92AA-D9ACB16D7C47}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -3177,12 +3177,20 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{310D2D95-3555-B746-82FE-2701FAF02A28}" name="Table3" displayName="Table3" ref="A1:J118" totalsRowShown="0">
   <autoFilter ref="A1:J118" xr:uid="{F5024BC6-9063-694A-A93E-42CCEC70DC0E}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Fer"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
   </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:J73">
+    <sortCondition ref="B1:B118"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{DF807125-8008-9B45-910F-BD5834AC4703}" name="Id " dataDxfId="1">
       <calculatedColumnFormula>ROW(Table3[[#This Row],[Id ]])-1</calculatedColumnFormula>
@@ -3513,8 +3521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4D1010-4D36-3C4D-9CF7-660420749DE7}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3531,61 +3539,61 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
         <v>87</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>90</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>91</v>
-      </c>
-      <c r="F1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" t="s">
-        <v>95</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
       </c>
       <c r="K1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F2" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -3594,28 +3602,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="F3" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -3624,28 +3632,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -3654,58 +3662,58 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="F6" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -3720,22 +3728,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F7" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -3750,22 +3758,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F8" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -3780,22 +3788,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -3810,22 +3818,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H10">
         <v>2</v>
@@ -3840,22 +3848,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="F11" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="G11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -3870,22 +3878,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="G12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H12">
         <v>3</v>
@@ -3900,28 +3908,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F13" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="G13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -3930,22 +3938,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="F14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -3960,22 +3968,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F15" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="G15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -3990,10 +3998,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -4002,10 +4010,10 @@
         <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="G16" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -4014,28 +4022,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>473</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>235</v>
+        <v>474</v>
       </c>
       <c r="F17" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="G17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H17">
         <v>3</v>
@@ -4044,58 +4052,58 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F18" t="s">
-        <v>134</v>
+        <v>472</v>
       </c>
       <c r="G18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F19" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -4104,568 +4112,568 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>353</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F20" t="s">
-        <v>222</v>
+        <v>468</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C21" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F21" t="s">
-        <v>223</v>
+        <v>146</v>
       </c>
       <c r="G21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>476</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>238</v>
+        <v>477</v>
       </c>
       <c r="F22" t="s">
-        <v>142</v>
-      </c>
-      <c r="G22" t="s">
-        <v>98</v>
+        <v>478</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="J22" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
         <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>146</v>
-      </c>
-      <c r="G23" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="J23" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>147</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>239</v>
+        <v>68</v>
       </c>
       <c r="F24" t="s">
-        <v>149</v>
-      </c>
-      <c r="G24" t="s">
-        <v>98</v>
+        <v>479</v>
       </c>
       <c r="H24">
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="J24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C25" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D25" t="s">
         <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F25" t="s">
+        <v>457</v>
+      </c>
+      <c r="G25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>152</v>
       </c>
-      <c r="G25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H25">
-        <v>3</v>
-      </c>
-      <c r="I25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>153</v>
-      </c>
-      <c r="C26" t="s">
-        <v>154</v>
       </c>
       <c r="D26" t="s">
         <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>351</v>
+        <v>231</v>
       </c>
       <c r="F26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G26" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H26">
         <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
         <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="F27" t="s">
-        <v>470</v>
+        <v>213</v>
       </c>
       <c r="G27" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C28" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="D28" t="s">
         <v>23</v>
       </c>
       <c r="E28" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F28" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="G28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>320</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>321</v>
       </c>
       <c r="D29" t="s">
         <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="F29" t="s">
-        <v>472</v>
-      </c>
-      <c r="G29" t="s">
-        <v>98</v>
+        <v>343</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+      <c r="J29" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>163</v>
+        <v>249</v>
       </c>
       <c r="C30" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
         <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="F30" t="s">
-        <v>468</v>
-      </c>
-      <c r="G30" t="s">
-        <v>98</v>
+        <v>250</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+      <c r="J30" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>165</v>
+        <v>323</v>
       </c>
       <c r="C31" t="s">
-        <v>366</v>
+        <v>324</v>
       </c>
       <c r="D31" t="s">
         <v>23</v>
       </c>
       <c r="E31" t="s">
-        <v>245</v>
+        <v>325</v>
       </c>
       <c r="F31" t="s">
-        <v>483</v>
-      </c>
-      <c r="G31" t="s">
-        <v>98</v>
+        <v>344</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+      <c r="J31" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D32" t="s">
         <v>23</v>
       </c>
       <c r="E32" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="F32" t="s">
-        <v>471</v>
+        <v>140</v>
       </c>
       <c r="G32" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="C33" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="D33" t="s">
         <v>23</v>
       </c>
       <c r="E33" t="s">
-        <v>171</v>
+        <v>228</v>
       </c>
       <c r="F33" t="s">
-        <v>473</v>
+        <v>143</v>
       </c>
       <c r="G33" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H33">
         <v>2</v>
       </c>
       <c r="I33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="D34" t="s">
         <v>23</v>
       </c>
       <c r="E34" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="F34" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="G34" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="D35" t="s">
         <v>23</v>
       </c>
       <c r="E35" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="F35" t="s">
-        <v>176</v>
+        <v>455</v>
       </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I35" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>177</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>178</v>
+        <v>353</v>
       </c>
       <c r="D36" t="s">
         <v>23</v>
       </c>
       <c r="E36" t="s">
-        <v>248</v>
+        <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>350</v>
-      </c>
-      <c r="G36" t="s">
-        <v>98</v>
+        <v>480</v>
       </c>
       <c r="H36">
         <v>2</v>
       </c>
       <c r="I36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="J36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>179</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="D37" t="s">
         <v>23</v>
       </c>
       <c r="E37" t="s">
-        <v>249</v>
+        <v>33</v>
       </c>
       <c r="F37" t="s">
-        <v>181</v>
-      </c>
-      <c r="G37" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="H37">
         <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="J37" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C38" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D38" t="s">
         <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="F38" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="G38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -4674,28 +4682,28 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C39" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D39" t="s">
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="F39" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="G39" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H39">
         <v>2</v>
@@ -4704,58 +4712,58 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="C40" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D40" t="s">
         <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="F40" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="G40" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C41" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="F41" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="G41" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -4764,13 +4772,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C42" t="s">
         <v>63</v>
@@ -4779,70 +4787,70 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="F42" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C43" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D43" t="s">
         <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="F43" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="G43" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C44" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D44" t="s">
         <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="F44" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="G44" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -4851,85 +4859,85 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="C45" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="D45" t="s">
         <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="F45" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="H45">
         <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D46" t="s">
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="F46" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="G46" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H46">
         <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C47" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D47" t="s">
         <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="F47" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="G47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H47">
         <v>2</v>
@@ -4938,88 +4946,88 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C48" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D48" t="s">
         <v>52</v>
       </c>
       <c r="E48" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="F48" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="G48" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H48">
         <v>2</v>
       </c>
       <c r="I48" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C49" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D49" t="s">
         <v>52</v>
       </c>
       <c r="E49" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="F49" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="G49" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H49">
         <v>2</v>
       </c>
       <c r="I49" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C50" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
       </c>
       <c r="E50" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="F50" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="G50" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H50">
         <v>2</v>
@@ -5028,28 +5036,28 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D51" t="s">
         <v>52</v>
       </c>
       <c r="E51" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="F51" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G51" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H51">
         <v>3</v>
@@ -5058,28 +5066,28 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C52" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D52" t="s">
         <v>52</v>
       </c>
       <c r="E52" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="F52" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="G52" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H52">
         <v>3</v>
@@ -5088,28 +5096,28 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C53" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D53" t="s">
         <v>52</v>
       </c>
       <c r="E53" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="F53" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="G53" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H53">
         <v>3</v>
@@ -5118,58 +5126,58 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C54" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D54" t="s">
         <v>52</v>
       </c>
       <c r="E54" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="F54" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="G54" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H54">
         <v>3</v>
       </c>
       <c r="I54" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C55" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D55" t="s">
         <v>52</v>
       </c>
       <c r="E55" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="F55" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G55" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H55">
         <v>3</v>
@@ -5178,13 +5186,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
@@ -5193,28 +5201,28 @@
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="F56" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="H56">
         <v>3</v>
       </c>
       <c r="I56" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="J56" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
@@ -5223,19 +5231,19 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="F57" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="H57">
         <v>2</v>
       </c>
       <c r="I57" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="J57" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -5244,7 +5252,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="C58" t="s">
         <v>37</v>
@@ -5253,19 +5261,19 @@
         <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="F58" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="H58">
         <v>3</v>
       </c>
       <c r="I58" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="J58" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -5274,28 +5282,28 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="C59" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="F59" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
       <c r="H59">
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="J59" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -5304,28 +5312,28 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="C60" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F60" t="s">
-        <v>323</v>
+        <v>487</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="J60" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -5334,28 +5342,28 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C61" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="F61" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="H61">
         <v>2</v>
       </c>
       <c r="I61" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="J61" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -5364,28 +5372,28 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="C62" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="F62" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="H62">
         <v>2</v>
       </c>
       <c r="I62" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="J62" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -5394,28 +5402,28 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="C63" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="F63" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="H63">
         <v>2</v>
       </c>
       <c r="I63" t="s">
+        <v>267</v>
+      </c>
+      <c r="J63" t="s">
         <v>278</v>
-      </c>
-      <c r="J63" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -5424,16 +5432,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="C64" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="F64" t="s">
         <v>28</v>
@@ -5442,79 +5450,79 @@
         <v>2</v>
       </c>
       <c r="I64" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="J64" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>332</v>
+        <v>132</v>
       </c>
       <c r="C65" t="s">
-        <v>333</v>
+        <v>118</v>
       </c>
       <c r="D65" t="s">
         <v>23</v>
       </c>
       <c r="E65" t="s">
-        <v>334</v>
+        <v>226</v>
       </c>
       <c r="F65" t="s">
-        <v>356</v>
+        <v>212</v>
+      </c>
+      <c r="G65" t="s">
+        <v>94</v>
       </c>
       <c r="H65">
         <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>269</v>
-      </c>
-      <c r="J65" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>335</v>
+        <v>150</v>
       </c>
       <c r="C66" t="s">
-        <v>336</v>
+        <v>151</v>
       </c>
       <c r="D66" t="s">
         <v>23</v>
       </c>
       <c r="E66" t="s">
-        <v>337</v>
+        <v>230</v>
       </c>
       <c r="F66" t="s">
-        <v>357</v>
+        <v>481</v>
+      </c>
+      <c r="G66" t="s">
+        <v>94</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I66" t="s">
-        <v>271</v>
-      </c>
-      <c r="J66" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -5523,208 +5531,208 @@
         <v>23</v>
       </c>
       <c r="E67" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="F67" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="J67" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>482</v>
       </c>
       <c r="C68" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="D68" t="s">
         <v>23</v>
       </c>
       <c r="E68" t="s">
+        <v>237</v>
+      </c>
+      <c r="F68" t="s">
+        <v>483</v>
+      </c>
+      <c r="G68" t="s">
+        <v>94</v>
+      </c>
+      <c r="H68">
+        <v>2</v>
+      </c>
+      <c r="I68" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>68</v>
       </c>
-      <c r="F68" t="s">
-        <v>69</v>
-      </c>
-      <c r="H68">
-        <v>3</v>
-      </c>
-      <c r="I68" t="s">
-        <v>70</v>
-      </c>
-      <c r="J68" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
-        <v>68</v>
-      </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>163</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>164</v>
       </c>
       <c r="D69" t="s">
         <v>23</v>
       </c>
       <c r="E69" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="F69" t="s">
-        <v>74</v>
+        <v>458</v>
+      </c>
+      <c r="G69" t="s">
+        <v>94</v>
       </c>
       <c r="H69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I69" t="s">
-        <v>75</v>
-      </c>
-      <c r="J69" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>76</v>
+        <v>170</v>
       </c>
       <c r="C70" t="s">
-        <v>77</v>
+        <v>171</v>
       </c>
       <c r="D70" t="s">
         <v>23</v>
       </c>
       <c r="E70" t="s">
-        <v>78</v>
+        <v>238</v>
       </c>
       <c r="F70" t="s">
+        <v>484</v>
+      </c>
+      <c r="G70" t="s">
+        <v>94</v>
+      </c>
+      <c r="H70">
+        <v>2</v>
+      </c>
+      <c r="I70" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>485</v>
+      </c>
+      <c r="C71" t="s">
         <v>166</v>
-      </c>
-      <c r="H70">
-        <v>3</v>
-      </c>
-      <c r="I70" t="s">
-        <v>79</v>
-      </c>
-      <c r="J70" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" t="s">
-        <v>32</v>
       </c>
       <c r="D71" t="s">
         <v>23</v>
       </c>
       <c r="E71" t="s">
-        <v>33</v>
+        <v>235</v>
       </c>
       <c r="F71" t="s">
-        <v>34</v>
+        <v>486</v>
+      </c>
+      <c r="G71" t="s">
+        <v>94</v>
       </c>
       <c r="H71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I71" t="s">
-        <v>35</v>
-      </c>
-      <c r="J71" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="C72" t="s">
-        <v>366</v>
+        <v>148</v>
       </c>
       <c r="D72" t="s">
         <v>23</v>
       </c>
       <c r="E72" t="s">
-        <v>27</v>
+        <v>338</v>
       </c>
       <c r="F72" t="s">
-        <v>486</v>
+        <v>149</v>
+      </c>
+      <c r="G72" t="s">
+        <v>94</v>
       </c>
       <c r="H72">
         <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>29</v>
-      </c>
-      <c r="J72" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>260</v>
+        <v>161</v>
       </c>
       <c r="C73" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="D73" t="s">
         <v>23</v>
       </c>
       <c r="E73" t="s">
-        <v>237</v>
+        <v>162</v>
       </c>
       <c r="F73" t="s">
-        <v>261</v>
+        <v>456</v>
+      </c>
+      <c r="G73" t="s">
+        <v>94</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
       <c r="I73" t="s">
-        <v>283</v>
-      </c>
-      <c r="J73" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C74" t="s">
         <v>12</v>
@@ -5733,29 +5741,29 @@
         <v>52</v>
       </c>
       <c r="E74" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F74" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="J74" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K74" s="3"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C75" t="s">
         <v>61</v>
@@ -5764,29 +5772,29 @@
         <v>52</v>
       </c>
       <c r="E75" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="F75" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="J75" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K75" s="3"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="C76" t="s">
         <v>61</v>
@@ -5795,29 +5803,29 @@
         <v>52</v>
       </c>
       <c r="E76" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="F76" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="J76" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K76" s="3"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C77" t="s">
         <v>51</v>
@@ -5826,28 +5834,28 @@
         <v>52</v>
       </c>
       <c r="E77" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="F77" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="J77" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="C78" t="s">
         <v>51</v>
@@ -5856,29 +5864,29 @@
         <v>52</v>
       </c>
       <c r="E78" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F78" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="J78" t="s">
+        <v>278</v>
+      </c>
+      <c r="K78" s="3"/>
+    </row>
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
         <v>289</v>
-      </c>
-      <c r="K78" s="3"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
-        <v>78</v>
-      </c>
-      <c r="B79" t="s">
-        <v>300</v>
       </c>
       <c r="C79" t="s">
         <v>63</v>
@@ -5887,125 +5895,125 @@
         <v>52</v>
       </c>
       <c r="E79" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="F79" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="H79">
         <v>2</v>
       </c>
       <c r="I79" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="J79" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K79" s="3"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="C80" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D80" t="s">
         <v>52</v>
       </c>
       <c r="E80" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="F80" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="H80">
         <v>3</v>
       </c>
       <c r="I80" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="J80" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K80" s="3"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="C81" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="D81" t="s">
         <v>52</v>
       </c>
       <c r="E81" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="F81" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="J81" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K81" s="3"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C82" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D82" t="s">
         <v>52</v>
       </c>
       <c r="E82" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F82" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="G82" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H82">
         <v>2</v>
       </c>
       <c r="I82" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J82" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K82" s="3"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="C83" t="s">
         <v>61</v>
@@ -6014,811 +6022,811 @@
         <v>52</v>
       </c>
       <c r="E83" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="F83" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="J83" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K83" s="3"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="C84" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D84" t="s">
         <v>52</v>
       </c>
       <c r="E84" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="F84" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="G84" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="J84" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K84" s="3"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="C85" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D85" t="s">
         <v>52</v>
       </c>
       <c r="E85" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="F85" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="G85" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="J85" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K85" s="3"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="C86" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D86" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E86" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="F86" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="H86">
         <v>2</v>
       </c>
       <c r="I86" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="J86" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K86" s="3"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="C87" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D87" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E87" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="F87" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="H87">
         <v>2</v>
       </c>
       <c r="I87" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="J87" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K87" s="3"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="C88" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D88" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E88" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="F88" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="H88">
         <v>2</v>
       </c>
       <c r="I88" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="J88" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="K88" s="3"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="C89" t="s">
+        <v>357</v>
+      </c>
+      <c r="D89" t="s">
+        <v>358</v>
+      </c>
+      <c r="E89" t="s">
+        <v>366</v>
+      </c>
+      <c r="F89" t="s">
         <v>370</v>
-      </c>
-      <c r="D89" t="s">
-        <v>371</v>
-      </c>
-      <c r="E89" t="s">
-        <v>379</v>
-      </c>
-      <c r="F89" t="s">
-        <v>383</v>
       </c>
       <c r="H89">
         <v>3</v>
       </c>
       <c r="I89" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="J89" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="C90" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D90" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E90" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="F90" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="H90">
         <v>2</v>
       </c>
       <c r="I90" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="J90" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="C91" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D91" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E91" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="F91" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="H91">
         <v>3</v>
       </c>
       <c r="I91" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="J91" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="C92" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D92" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E92" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="F92" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="H92">
         <v>3</v>
       </c>
       <c r="I92" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="J92" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="C93" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D93" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E93" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="F93" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="H93">
         <v>3</v>
       </c>
       <c r="I93" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="J93" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="C94" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D94" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E94" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="F94" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="H94">
         <v>3</v>
       </c>
       <c r="I94" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="J94" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="C95" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D95" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E95" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="F95" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="J95" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="C96" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D96" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E96" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="F96" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="H96">
         <v>2</v>
       </c>
       <c r="I96" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="J96" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="C97" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D97" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E97" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="F97" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="H97">
         <v>3</v>
       </c>
       <c r="I97" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="J97" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="C98" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D98" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E98" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="F98" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="H98">
         <v>2</v>
       </c>
       <c r="I98" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="J98" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="C99" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D99" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E99" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="F99" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="H99">
         <v>2</v>
       </c>
       <c r="I99" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="J99" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="C100" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D100" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E100" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="F100" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="H100">
         <v>3</v>
       </c>
       <c r="I100" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="J100" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="C101" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D101" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E101" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="F101" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="H101">
         <v>2</v>
       </c>
       <c r="I101" t="s">
+        <v>399</v>
+      </c>
+      <c r="J101" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
         <v>412</v>
       </c>
-      <c r="J101" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <f>ROW(Table3[[#This Row],[Id ]])-1</f>
-        <v>101</v>
-      </c>
-      <c r="B102" t="s">
-        <v>425</v>
-      </c>
       <c r="C102" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D102" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E102" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="F102" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="H102">
         <v>3</v>
       </c>
       <c r="I102" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="J102" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="C103" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D103" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E103" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="F103" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="H103">
         <v>3</v>
       </c>
       <c r="I103" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="J103" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="C104" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D104" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E104" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="F104" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="H104">
         <v>2</v>
       </c>
       <c r="I104" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="J104" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="C105" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D105" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E105" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="F105" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="H105">
         <v>3</v>
       </c>
       <c r="I105" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="J105" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="C106" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D106" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E106" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="F106" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="H106">
         <v>3</v>
       </c>
       <c r="I106" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="J106" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="C107" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D107" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E107" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="F107" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="H107">
         <v>1</v>
       </c>
       <c r="I107" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="J107" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="C108" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D108" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E108" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="F108" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="H108">
         <v>3</v>
       </c>
       <c r="I108" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="J108" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C109" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D109" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E109" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F109" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="J109" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -6874,10 +6882,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B1" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -6909,7 +6917,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -6918,7 +6926,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -6954,7 +6962,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7008,7 +7016,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B16" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7044,7 +7052,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7053,7 +7061,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7062,7 +7070,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7071,7 +7079,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7080,7 +7088,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B24" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7089,7 +7097,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B25" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7098,7 +7106,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B26" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7116,7 +7124,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="B28" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7179,7 +7187,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="B35" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7188,7 +7196,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="B36" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7215,7 +7223,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B39" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7224,7 +7232,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B40" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7233,7 +7241,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="B41" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7269,7 +7277,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B45" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7278,7 +7286,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B46" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7296,7 +7304,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="B48" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7305,7 +7313,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="B49" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7323,7 +7331,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B51" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7332,7 +7340,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B52" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7341,7 +7349,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="B53" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7359,7 +7367,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="B55" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7377,7 +7385,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="B57" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7431,7 +7439,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="B63" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7440,7 +7448,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="B64" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7485,7 +7493,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="B69" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7503,7 +7511,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="B71" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7521,7 +7529,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="B73" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7548,7 +7556,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B76" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7566,7 +7574,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B78" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7584,7 +7592,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B80" s="3" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7602,7 +7610,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B82" s="3" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7611,7 +7619,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="B83" s="3" t="e">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7620,7 +7628,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="B84" s="3" t="e">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7654,18 +7662,18 @@
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -7677,7 +7685,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -7766,7 +7774,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -7776,7 +7784,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -7794,7 +7802,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3">

</xml_diff>

<commit_message>
Version created for lasercutting. Update in some characters names.
Increased bleed to help lasercut work fine
</commit_message>
<xml_diff>
--- a/src/resources/horde_cards.xlsx
+++ b/src/resources/horde_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsaban/git/perso/windwalkers-cardgame/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCC90BB-55D2-BB44-878B-A1C4467B6CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D693B6-560D-3945-8BE6-F5515A6E55C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{2F94C834-2D3B-4040-A9EF-5D9A64AD9988}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -257,9 +257,6 @@
     <t>Iphaine.png</t>
   </si>
   <si>
-    <t>Amonmas Amon</t>
-  </si>
-  <si>
     <t>ferrailleur</t>
   </si>
   <si>
@@ -362,9 +359,6 @@
     <t xml:space="preserve">scribe </t>
   </si>
   <si>
-    <t xml:space="preserve">Walo Waldmann </t>
-  </si>
-  <si>
     <t xml:space="preserve">protecteur </t>
   </si>
   <si>
@@ -380,27 +374,12 @@
     <t xml:space="preserve">τ:Ignorez les malus du terrain </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypekelus </t>
-  </si>
-  <si>
     <t xml:space="preserve">pilier </t>
   </si>
   <si>
-    <t xml:space="preserve">Thoratos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thoratos est capable de faire des miracles mais il a toujours eu besoin du soutien d'Hypekelus. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Athinatos Catanus </t>
-  </si>
-  <si>
     <t xml:space="preserve">ailier </t>
   </si>
   <si>
-    <t xml:space="preserve">La famille Catanus est celebre dans le pays pour la force et l'audace de ses membres. Athinatos n'y fait pas exception. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Blanchette de Gaude </t>
   </si>
   <si>
@@ -437,12 +416,6 @@
     <t xml:space="preserve">Oshora aime le silence et les huis-clos. C'est quand le groupe est petit qu'elle peut s'exprimer le mieux </t>
   </si>
   <si>
-    <t xml:space="preserve">Khypico Torantor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bepphon Torantor </t>
-  </si>
-  <si>
     <t xml:space="preserve">Gianni Raymondi </t>
   </si>
   <si>
@@ -461,9 +434,6 @@
     <t xml:space="preserve">Vif et surprenant sont les meilleurs qualificatifs pour Ernest. Il trouve toujours le meilleur chemin pour faire progresser le groupe. </t>
   </si>
   <si>
-    <t xml:space="preserve">τ:Devoilez le vent de 2 tuiles adjacente a votre tuile </t>
-  </si>
-  <si>
     <t xml:space="preserve">Galas Thunderflayer </t>
   </si>
   <si>
@@ -512,9 +482,6 @@
     <t xml:space="preserve">feuleuse </t>
   </si>
   <si>
-    <t xml:space="preserve">Ivo Baumann </t>
-  </si>
-  <si>
     <t xml:space="preserve">artisan du bois </t>
   </si>
   <si>
@@ -542,9 +509,6 @@
     <t xml:space="preserve">archere </t>
   </si>
   <si>
-    <t xml:space="preserve">Bertram Haring </t>
-  </si>
-  <si>
     <t xml:space="preserve">τ:Baissez la force du vent de 1 </t>
   </si>
   <si>
@@ -701,15 +665,9 @@
     <t xml:space="preserve">La discipline est le maitre mot d'Ukkiba. Ukkiba sait trouver les mots qu'il faut pour faire progresser le groupe. Même si ses mots sont durs. </t>
   </si>
   <si>
-    <t xml:space="preserve">Walo a toujours eu le sens de l'esquive. Il sait quand il est opportun de faire un pas de côté pour progresser. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Filibert lit le terrain comme on lit un livre d'enfant Il trouve des solutions à chaque nouveau danger, même les plus mortels. </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypekelus est un grand frère aimant qui a toujours vu loin. Sa grande taille lui permet de voir plus loin que les autres. </t>
-  </si>
-  <si>
     <t xml:space="preserve">On peut être une princesse et faire face à des tempêtes. </t>
   </si>
   <si>
@@ -740,18 +698,12 @@
     <t xml:space="preserve">Rien n'est plus important qu'un feu. Lorsque les os sont gelés, lorsque la peau est trempée, lorsque les ventres sont vides. </t>
   </si>
   <si>
-    <t xml:space="preserve">Tour à tour menuisier ébéniste luthier et musicien, Ivo sait réparer les outils meubles et les esprits. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Adolar commande et l'oiseau obéit. </t>
   </si>
   <si>
     <t xml:space="preserve">Saskia chasse le cerf et le sanglier. La foret est son terrain de prédilection. </t>
   </si>
   <si>
-    <t xml:space="preserve">Les montagnes ont des secrets que Bertram sait exploiter. Il voit dans le schiste les fractures et décèle les grottes a des kilomètres. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Si vous avez le vertige sur les corniches escarpées vous n'arriverez pas à le suivre. N'ayez crainte, Oliver sera là pour vous assurer. </t>
   </si>
   <si>
@@ -788,9 +740,6 @@
     <t>τ:Deplacez vous dans le sens du vent. Perdez 1 point de moral.</t>
   </si>
   <si>
-    <t>Elmeth Torantor</t>
-  </si>
-  <si>
     <t>τ:Lancez 1d6 supplementaire; gagnez 1 point de moral si vous avez un autre Torantor</t>
   </si>
   <si>
@@ -1019,12 +968,6 @@
     <t>Emelyn se fait discrete. Elle se fond au milieu du pack pour agir en toute discretion.</t>
   </si>
   <si>
-    <t>Noggangrid Ingotshield</t>
-  </si>
-  <si>
-    <t>Noggangrid est une mangeuse de livre. Certains disent qu'elles les auraient tous lu.</t>
-  </si>
-  <si>
     <t>τ:Abandonnez-la et regagnez 2 points de moral. Abandonnez le avec Pere et regagnez tout votre moral</t>
   </si>
   <si>
@@ -1358,9 +1301,6 @@
     <t>Kon bouge et tourne pour proteger son groupe. Attentif aux dangers, il protege et soutien sa horde.</t>
   </si>
   <si>
-    <t>τ:Abandonnez un Hordier du FER s'il n'est pas Calsan et recrutez un Calsan. Faites +/-1 par Calsan</t>
-  </si>
-  <si>
     <t xml:space="preserve">τ:Abandonnez-le et lancez autant de d6 que de Hordiers du FER </t>
   </si>
   <si>
@@ -1442,9 +1382,6 @@
     <t xml:space="preserve">τ:Perdez 1 point de moral. Appliquez +/-1 pour chaque points de moral sur vos d6 </t>
   </si>
   <si>
-    <t xml:space="preserve">τ:Echangez 2 tuiles sans nom et adjacentes. Perdez 1 point de moral sauf si Hypekelus est avec vous </t>
-  </si>
-  <si>
     <t>τ:Abandonnez un hordier de TRAINE. N'appliquez pas son pouvoir. Remplacez le par votre Faucon.</t>
   </si>
   <si>
@@ -1503,6 +1440,69 @@
   </si>
   <si>
     <t>τ:Piochez une carte consommable ou marquez un point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herbert est un grand frère aimant qui a toujours vu loin. Sa grande taille lui permet de voir plus loin que les autres. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franck est capable de faire des miracles mais il a toujours eu besoin du soutien de Franck. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">τ:Echangez 2 tuiles sans nom et adjacentes. Perdez 1 point de moral sauf si Herbert est avec vous </t>
+  </si>
+  <si>
+    <t>Athonios Catan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La famille Catan est celebre dans le pays pour la force et l'audace de ses membres. Athonios n'y fait pas exception. </t>
+  </si>
+  <si>
+    <t>τ:Abandonnez un Hordier du FER s'il n'est pas Calsan et recrutez un Calsan. Faites +/-1 par Hordier manquant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les montagnes ont des secrets que Bert sait exploiter. Il voit dans le schiste les fractures et décèle les grottes a des kilomètres. </t>
+  </si>
+  <si>
+    <t>Yavo Torantor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xavio Torantor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyo Torantor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivan Baumann </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tour à tour menuisier ébéniste luthier et musicien, Ivan sait réparer les outils meubles et les esprits. </t>
+  </si>
+  <si>
+    <t>Nadia Ingot</t>
+  </si>
+  <si>
+    <t>Nadia est une mangeuse de livre. Certains disent qu'elles les auraient tous lu.</t>
+  </si>
+  <si>
+    <t>Amon Amon</t>
+  </si>
+  <si>
+    <t>Herbert Benegh</t>
+  </si>
+  <si>
+    <t>Franck Benegh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waldo Waldmann </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waldo a toujours eu le sens de l'esquive. Il sait quand il est opportun de faire un pas de côté pour progresser. </t>
+  </si>
+  <si>
+    <t>τ:Devoilez le vent de 2 tuiles adjacentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bert Haring </t>
   </si>
 </sst>
 </file>
@@ -3070,7 +3070,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4C07DF30-360B-9D4E-92AA-D9ACB16D7C47}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4C07DF30-360B-9D4E-92AA-D9ACB16D7C47}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -3177,11 +3177,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{310D2D95-3555-B746-82FE-2701FAF02A28}" name="Table3" displayName="Table3" ref="A1:J118" totalsRowShown="0">
   <autoFilter ref="A1:J118" xr:uid="{F5024BC6-9063-694A-A93E-42CCEC70DC0E}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Fer"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3521,8 +3516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4D1010-4D36-3C4D-9CF7-660420749DE7}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3539,61 +3534,61 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>90</v>
-      </c>
-      <c r="I1" t="s">
-        <v>91</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
       </c>
       <c r="K1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="F2" t="s">
-        <v>454</v>
+        <v>434</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -3602,28 +3597,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
         <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>96</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="F3" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -3632,28 +3627,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" t="s">
         <v>98</v>
       </c>
-      <c r="F4" t="s">
-        <v>99</v>
-      </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -3662,58 +3657,58 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="F6" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -3728,22 +3723,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
         <v>103</v>
-      </c>
-      <c r="C7" t="s">
-        <v>104</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F7" t="s">
-        <v>451</v>
+        <v>431</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -3758,22 +3753,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="s">
         <v>105</v>
-      </c>
-      <c r="C8" t="s">
-        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="F8" t="s">
-        <v>466</v>
+        <v>446</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -3788,22 +3783,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>484</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>220</v>
+        <v>485</v>
       </c>
       <c r="F9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -3818,25 +3813,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="F10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10" t="s">
         <v>11</v>
@@ -3848,22 +3843,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>482</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>222</v>
+        <v>467</v>
       </c>
       <c r="F11" t="s">
-        <v>435</v>
+        <v>416</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -3878,22 +3873,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>483</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>468</v>
       </c>
       <c r="F12" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H12">
         <v>3</v>
@@ -3908,28 +3903,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>470</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>119</v>
+        <v>471</v>
       </c>
       <c r="F13" t="s">
-        <v>452</v>
+        <v>432</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -3938,22 +3933,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -3968,22 +3963,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="F15" t="s">
-        <v>453</v>
+        <v>433</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -3998,10 +3993,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -4010,10 +4005,10 @@
         <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -4028,25 +4023,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="F17" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I17" t="s">
         <v>20</v>
@@ -4058,22 +4053,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="F18" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H18">
         <v>2</v>
@@ -4088,22 +4083,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F19" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -4112,28 +4107,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H20">
         <v>3</v>
@@ -4142,28 +4137,28 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D21" t="s">
         <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="F21" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H21">
         <v>3</v>
@@ -4172,13 +4167,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="C22" t="s">
         <v>70</v>
@@ -4187,10 +4182,10 @@
         <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
       <c r="F22" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
       <c r="H22">
         <v>3</v>
@@ -4199,40 +4194,40 @@
         <v>71</v>
       </c>
       <c r="J22" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>481</v>
+      </c>
+      <c r="C23" t="s">
         <v>72</v>
-      </c>
-      <c r="C23" t="s">
-        <v>73</v>
       </c>
       <c r="D23" t="s">
         <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="H23">
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J23" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>23</v>
@@ -4250,7 +4245,7 @@
         <v>68</v>
       </c>
       <c r="F24" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="H24">
         <v>2</v>
@@ -4259,31 +4254,31 @@
         <v>69</v>
       </c>
       <c r="J24" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C25" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
         <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="F25" t="s">
-        <v>457</v>
+        <v>437</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H25">
         <v>2</v>
@@ -4292,28 +4287,28 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D26" t="s">
         <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="F26" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H26">
         <v>2</v>
@@ -4322,28 +4317,28 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>475</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D27" t="s">
         <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F27" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -4352,73 +4347,73 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>167</v>
+        <v>487</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D28" t="s">
         <v>23</v>
       </c>
       <c r="E28" t="s">
-        <v>236</v>
+        <v>473</v>
       </c>
       <c r="F28" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="C29" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="D29" t="s">
         <v>23</v>
       </c>
       <c r="E29" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="F29" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="J29" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>249</v>
+        <v>474</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -4427,73 +4422,73 @@
         <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F30" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="J30" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="C31" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="D31" t="s">
         <v>23</v>
       </c>
       <c r="E31" t="s">
+        <v>308</v>
+      </c>
+      <c r="F31" t="s">
         <v>325</v>
-      </c>
-      <c r="F31" t="s">
-        <v>344</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="J31" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D32" t="s">
         <v>23</v>
       </c>
       <c r="E32" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F32" t="s">
-        <v>140</v>
+        <v>486</v>
       </c>
       <c r="G32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -4502,28 +4497,28 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D33" t="s">
         <v>23</v>
       </c>
       <c r="E33" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="F33" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="G33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -4532,28 +4527,28 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D34" t="s">
         <v>23</v>
       </c>
       <c r="E34" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="F34" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -4562,28 +4557,28 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>477</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D35" t="s">
         <v>23</v>
       </c>
       <c r="E35" t="s">
-        <v>233</v>
+        <v>478</v>
       </c>
       <c r="F35" t="s">
-        <v>455</v>
+        <v>435</v>
       </c>
       <c r="G35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -4592,7 +4587,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>35</v>
@@ -4601,7 +4596,7 @@
         <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="D36" t="s">
         <v>23</v>
@@ -4610,7 +4605,7 @@
         <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -4619,10 +4614,10 @@
         <v>29</v>
       </c>
       <c r="J36" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>36</v>
@@ -4649,31 +4644,31 @@
         <v>35</v>
       </c>
       <c r="J37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D38" t="s">
         <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="F38" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="G38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -4682,28 +4677,28 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C39" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D39" t="s">
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="F39" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="G39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H39">
         <v>2</v>
@@ -4712,58 +4707,58 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="C40" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D40" t="s">
         <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="F40" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="G40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C41" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F41" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="G41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -4772,13 +4767,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="C42" t="s">
         <v>63</v>
@@ -4787,70 +4782,70 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="F42" t="s">
-        <v>459</v>
+        <v>439</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D43" t="s">
         <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="F43" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="G43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D44" t="s">
         <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="F44" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="G44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -4859,85 +4854,85 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="C45" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="D45" t="s">
         <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="F45" t="s">
-        <v>448</v>
+        <v>428</v>
       </c>
       <c r="H45">
         <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C46" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D46" t="s">
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="F46" t="s">
-        <v>449</v>
+        <v>429</v>
       </c>
       <c r="G46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H46">
         <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C47" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D47" t="s">
         <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="F47" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="G47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H47">
         <v>2</v>
@@ -4946,88 +4941,88 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C48" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D48" t="s">
         <v>52</v>
       </c>
       <c r="E48" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="F48" t="s">
-        <v>450</v>
+        <v>430</v>
       </c>
       <c r="G48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H48">
         <v>2</v>
       </c>
       <c r="I48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D49" t="s">
         <v>52</v>
       </c>
       <c r="E49" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="F49" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="G49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H49">
         <v>2</v>
       </c>
       <c r="I49" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C50" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D50" t="s">
         <v>52</v>
       </c>
       <c r="E50" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="F50" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="G50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H50">
         <v>2</v>
@@ -5036,28 +5031,28 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="C51" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D51" t="s">
         <v>52</v>
       </c>
       <c r="E51" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="F51" t="s">
-        <v>460</v>
+        <v>440</v>
       </c>
       <c r="G51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H51">
         <v>3</v>
@@ -5066,28 +5061,28 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="C52" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D52" t="s">
         <v>52</v>
       </c>
       <c r="E52" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="F52" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H52">
         <v>3</v>
@@ -5096,28 +5091,28 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C53" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D53" t="s">
         <v>52</v>
       </c>
       <c r="E53" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="F53" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="G53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H53">
         <v>3</v>
@@ -5126,58 +5121,58 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C54" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D54" t="s">
         <v>52</v>
       </c>
       <c r="E54" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="F54" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="G54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H54">
         <v>3</v>
       </c>
       <c r="I54" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C55" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D55" t="s">
         <v>52</v>
       </c>
       <c r="E55" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="F55" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="G55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H55">
         <v>3</v>
@@ -5186,13 +5181,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
@@ -5201,28 +5196,28 @@
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="F56" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="H56">
         <v>3</v>
       </c>
       <c r="I56" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="J56" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
@@ -5231,19 +5226,19 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="F57" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
       <c r="H57">
         <v>2</v>
       </c>
       <c r="I57" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="J57" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -5252,7 +5247,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="C58" t="s">
         <v>37</v>
@@ -5261,19 +5256,19 @@
         <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="F58" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="H58">
         <v>3</v>
       </c>
       <c r="I58" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="J58" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
@@ -5282,28 +5277,28 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="C59" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="F59" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="H59">
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="J59" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
@@ -5312,28 +5307,28 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="C60" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="F60" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="J60" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -5342,28 +5337,28 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="C61" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="F61" t="s">
-        <v>439</v>
+        <v>472</v>
       </c>
       <c r="H61">
         <v>2</v>
       </c>
       <c r="I61" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="J61" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
@@ -5372,28 +5367,28 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="C62" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="F62" t="s">
-        <v>462</v>
+        <v>442</v>
       </c>
       <c r="H62">
         <v>2</v>
       </c>
       <c r="I62" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="J62" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
@@ -5402,28 +5397,28 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="C63" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="F63" t="s">
-        <v>461</v>
+        <v>441</v>
       </c>
       <c r="H63">
         <v>2</v>
       </c>
       <c r="I63" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="J63" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
@@ -5432,16 +5427,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>436</v>
+        <v>417</v>
       </c>
       <c r="C64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>438</v>
+        <v>419</v>
       </c>
       <c r="F64" t="s">
         <v>28</v>
@@ -5450,34 +5445,34 @@
         <v>2</v>
       </c>
       <c r="I64" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="J64" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>476</v>
       </c>
       <c r="C65" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D65" t="s">
         <v>23</v>
       </c>
       <c r="E65" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F65" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="G65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -5486,28 +5481,28 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C66" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D66" t="s">
         <v>23</v>
       </c>
       <c r="E66" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="F66" t="s">
-        <v>481</v>
+        <v>460</v>
       </c>
       <c r="G66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H66">
         <v>3</v>
@@ -5516,13 +5511,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>326</v>
+        <v>479</v>
       </c>
       <c r="C67" t="s">
         <v>17</v>
@@ -5531,43 +5526,43 @@
         <v>23</v>
       </c>
       <c r="E67" t="s">
-        <v>327</v>
+        <v>480</v>
       </c>
       <c r="F67" t="s">
-        <v>463</v>
+        <v>443</v>
       </c>
       <c r="H67">
         <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="J67" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>482</v>
+        <v>461</v>
       </c>
       <c r="C68" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D68" t="s">
         <v>23</v>
       </c>
       <c r="E68" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="F68" t="s">
-        <v>483</v>
+        <v>462</v>
       </c>
       <c r="G68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H68">
         <v>2</v>
@@ -5576,28 +5571,28 @@
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C69" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D69" t="s">
         <v>23</v>
       </c>
       <c r="E69" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F69" t="s">
-        <v>458</v>
+        <v>438</v>
       </c>
       <c r="G69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H69">
         <v>2</v>
@@ -5606,28 +5601,28 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C70" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="D70" t="s">
         <v>23</v>
       </c>
       <c r="E70" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="F70" t="s">
-        <v>484</v>
+        <v>463</v>
       </c>
       <c r="G70" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H70">
         <v>2</v>
@@ -5636,28 +5631,28 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>485</v>
+        <v>464</v>
       </c>
       <c r="C71" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D71" t="s">
         <v>23</v>
       </c>
       <c r="E71" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="F71" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
       <c r="G71" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H71">
         <v>3</v>
@@ -5666,28 +5661,28 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C72" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D72" t="s">
         <v>23</v>
       </c>
       <c r="E72" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="F72" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="G72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H72">
         <v>2</v>
@@ -5696,28 +5691,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D73" t="s">
         <v>23</v>
       </c>
       <c r="E73" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="F73" t="s">
-        <v>456</v>
+        <v>436</v>
       </c>
       <c r="G73" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -5726,13 +5721,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="C74" t="s">
         <v>12</v>
@@ -5741,29 +5736,29 @@
         <v>52</v>
       </c>
       <c r="E74" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="F74" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="J74" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K74" s="3"/>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="C75" t="s">
         <v>61</v>
@@ -5772,29 +5767,29 @@
         <v>52</v>
       </c>
       <c r="E75" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F75" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="J75" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K75" s="3"/>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="C76" t="s">
         <v>61</v>
@@ -5803,29 +5798,29 @@
         <v>52</v>
       </c>
       <c r="E76" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F76" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="J76" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K76" s="3"/>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="C77" t="s">
         <v>51</v>
@@ -5834,28 +5829,28 @@
         <v>52</v>
       </c>
       <c r="E77" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="F77" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="J77" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="C78" t="s">
         <v>51</v>
@@ -5864,29 +5859,29 @@
         <v>52</v>
       </c>
       <c r="E78" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="F78" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
       <c r="I78" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="J78" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K78" s="3"/>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="C79" t="s">
         <v>63</v>
@@ -5895,125 +5890,125 @@
         <v>52</v>
       </c>
       <c r="E79" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="F79" t="s">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="H79">
         <v>2</v>
       </c>
       <c r="I79" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="J79" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K79" s="3"/>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="C80" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="D80" t="s">
         <v>52</v>
       </c>
       <c r="E80" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="F80" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="H80">
         <v>3</v>
       </c>
       <c r="I80" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="J80" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K80" s="3"/>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="C81" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="D81" t="s">
         <v>52</v>
       </c>
       <c r="E81" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="F81" t="s">
-        <v>465</v>
+        <v>445</v>
       </c>
       <c r="H81">
         <v>1</v>
       </c>
       <c r="I81" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="J81" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K81" s="3"/>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C82" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D82" t="s">
         <v>52</v>
       </c>
       <c r="E82" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="F82" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="G82" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H82">
         <v>2</v>
       </c>
       <c r="I82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J82" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K82" s="3"/>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="C83" t="s">
         <v>61</v>
@@ -6022,811 +6017,811 @@
         <v>52</v>
       </c>
       <c r="E83" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="F83" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="H83">
         <v>1</v>
       </c>
       <c r="I83" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="J83" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K83" s="3"/>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>443</v>
+        <v>423</v>
       </c>
       <c r="C84" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D84" t="s">
         <v>52</v>
       </c>
       <c r="E84" t="s">
-        <v>444</v>
+        <v>424</v>
       </c>
       <c r="F84" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="G84" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H84">
         <v>1</v>
       </c>
       <c r="I84" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="J84" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K84" s="3"/>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="C85" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D85" t="s">
         <v>52</v>
       </c>
       <c r="E85" t="s">
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="F85" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
       <c r="G85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H85">
         <v>1</v>
       </c>
       <c r="I85" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="J85" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K85" s="3"/>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>356</v>
+        <v>337</v>
       </c>
       <c r="C86" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D86" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E86" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
       <c r="F86" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="H86">
         <v>2</v>
       </c>
       <c r="I86" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="J86" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K86" s="3"/>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="C87" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D87" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E87" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="F87" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="H87">
         <v>2</v>
       </c>
       <c r="I87" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="J87" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K87" s="3"/>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="C88" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D88" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E88" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="F88" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="H88">
         <v>2</v>
       </c>
       <c r="I88" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="J88" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K88" s="3"/>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="C89" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D89" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E89" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="F89" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
       <c r="H89">
         <v>3</v>
       </c>
       <c r="I89" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="J89" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="C90" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D90" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E90" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
       <c r="F90" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="H90">
         <v>2</v>
       </c>
       <c r="I90" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="J90" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="C91" t="s">
+        <v>338</v>
+      </c>
+      <c r="D91" t="s">
+        <v>339</v>
+      </c>
+      <c r="E91" t="s">
         <v>357</v>
       </c>
-      <c r="D91" t="s">
+      <c r="F91" t="s">
         <v>358</v>
-      </c>
-      <c r="E91" t="s">
-        <v>376</v>
-      </c>
-      <c r="F91" t="s">
-        <v>377</v>
       </c>
       <c r="H91">
         <v>3</v>
       </c>
       <c r="I91" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="J91" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>378</v>
+        <v>359</v>
       </c>
       <c r="C92" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D92" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E92" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
       <c r="F92" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="H92">
         <v>3</v>
       </c>
       <c r="I92" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="J92" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="C93" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D93" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E93" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
       <c r="F93" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="H93">
         <v>3</v>
       </c>
       <c r="I93" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="J93" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="C94" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D94" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E94" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="F94" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
       <c r="H94">
         <v>3</v>
       </c>
       <c r="I94" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="J94" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>388</v>
+        <v>369</v>
       </c>
       <c r="C95" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D95" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E95" t="s">
-        <v>389</v>
+        <v>370</v>
       </c>
       <c r="F95" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="H95">
         <v>1</v>
       </c>
       <c r="I95" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="J95" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="C96" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D96" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E96" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
       <c r="F96" t="s">
-        <v>394</v>
+        <v>375</v>
       </c>
       <c r="H96">
         <v>2</v>
       </c>
       <c r="I96" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="J96" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>396</v>
+        <v>377</v>
       </c>
       <c r="C97" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D97" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E97" t="s">
-        <v>397</v>
+        <v>378</v>
       </c>
       <c r="F97" t="s">
-        <v>398</v>
+        <v>379</v>
       </c>
       <c r="H97">
         <v>3</v>
       </c>
       <c r="I97" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="J97" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
       <c r="C98" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D98" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E98" t="s">
-        <v>401</v>
+        <v>382</v>
       </c>
       <c r="F98" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="H98">
         <v>2</v>
       </c>
       <c r="I98" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="J98" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="C99" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D99" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E99" t="s">
-        <v>404</v>
+        <v>385</v>
       </c>
       <c r="F99" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="H99">
         <v>2</v>
       </c>
       <c r="I99" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="J99" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="C100" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D100" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E100" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="F100" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
       <c r="H100">
         <v>3</v>
       </c>
       <c r="I100" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="J100" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>409</v>
+        <v>390</v>
       </c>
       <c r="C101" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D101" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E101" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="F101" t="s">
-        <v>411</v>
+        <v>392</v>
       </c>
       <c r="H101">
         <v>2</v>
       </c>
       <c r="I101" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="J101" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>412</v>
+        <v>393</v>
       </c>
       <c r="C102" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D102" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E102" t="s">
-        <v>413</v>
+        <v>394</v>
       </c>
       <c r="F102" t="s">
-        <v>414</v>
+        <v>395</v>
       </c>
       <c r="H102">
         <v>3</v>
       </c>
       <c r="I102" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
       <c r="J102" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="C103" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D103" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E103" t="s">
-        <v>417</v>
+        <v>398</v>
       </c>
       <c r="F103" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="H103">
         <v>3</v>
       </c>
       <c r="I103" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
       <c r="J103" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="C104" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D104" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E104" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
       <c r="F104" t="s">
-        <v>421</v>
+        <v>402</v>
       </c>
       <c r="H104">
         <v>2</v>
       </c>
       <c r="I104" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="J104" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>422</v>
+        <v>403</v>
       </c>
       <c r="C105" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D105" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E105" t="s">
-        <v>423</v>
+        <v>404</v>
       </c>
       <c r="F105" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
       <c r="H105">
         <v>3</v>
       </c>
       <c r="I105" t="s">
-        <v>425</v>
+        <v>406</v>
       </c>
       <c r="J105" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>426</v>
+        <v>407</v>
       </c>
       <c r="C106" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D106" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E106" t="s">
-        <v>427</v>
+        <v>408</v>
       </c>
       <c r="F106" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
       <c r="H106">
         <v>3</v>
       </c>
       <c r="I106" t="s">
-        <v>425</v>
+        <v>406</v>
       </c>
       <c r="J106" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="C107" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D107" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E107" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="F107" t="s">
-        <v>431</v>
+        <v>412</v>
       </c>
       <c r="H107">
         <v>1</v>
       </c>
       <c r="I107" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
       <c r="J107" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="C108" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D108" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E108" t="s">
-        <v>433</v>
+        <v>414</v>
       </c>
       <c r="F108" t="s">
-        <v>434</v>
+        <v>415</v>
       </c>
       <c r="H108">
         <v>3</v>
       </c>
       <c r="I108" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="J108" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C109" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D109" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="E109" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F109" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="J109" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
     <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -6882,10 +6877,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="B1" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -6917,7 +6912,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -6926,7 +6921,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>330</v>
+        <v>311</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -6962,7 +6957,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7016,7 +7011,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="B16" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7052,7 +7047,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7061,7 +7056,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7070,7 +7065,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7079,7 +7074,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7088,7 +7083,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7097,7 +7092,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="B25" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7106,7 +7101,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7124,7 +7119,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="B28" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7187,7 +7182,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="B35" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7196,7 +7191,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="B36" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7223,7 +7218,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="B39" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7241,7 +7236,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="B41" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7277,7 +7272,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7286,7 +7281,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="B46" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7304,7 +7299,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="B48" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7313,7 +7308,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="B49" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7331,7 +7326,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="B51" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7349,7 +7344,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="B53" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7367,7 +7362,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="B55" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7385,7 +7380,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="B57" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7439,7 +7434,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="B63" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7448,7 +7443,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="B64" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7493,7 +7488,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="B69" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7511,7 +7506,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="B71" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7529,7 +7524,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="B73" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7556,7 +7551,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="B76" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7574,7 +7569,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="B78" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7592,7 +7587,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="B80" s="3" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7610,7 +7605,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="3" t="str">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7619,7 +7614,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="B83" s="3" t="e">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7628,7 +7623,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="B84" s="3" t="e">
         <f>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</f>
@@ -7662,18 +7657,18 @@
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -7685,7 +7680,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -7774,7 +7769,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -7784,7 +7779,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -7802,7 +7797,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3">

</xml_diff>

<commit_message>
compass and grey borders
</commit_message>
<xml_diff>
--- a/src/resources/horde_cards.xlsx
+++ b/src/resources/horde_cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsaban/git/perso/windwalkers-cardgame/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90F3EC4-98A3-EC48-B414-743D6F832414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC85CA59-4782-2140-BA22-C2E9E182004D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1280" windowWidth="27540" windowHeight="15340" activeTab="1" xr2:uid="{2F94C834-2D3B-4040-A9EF-5D9A64AD9988}"/>
+    <workbookView xWindow="940" yWindow="1280" windowWidth="27540" windowHeight="15340" xr2:uid="{2F94C834-2D3B-4040-A9EF-5D9A64AD9988}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId6"/>
+    <pivotCache cacheId="8" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2809,7 +2809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2822,42 +2822,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="34">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFD4D4D4"/>
-        <name val="Menlo"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -3080,6 +3049,31 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <name val="Menlo"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -5889,7 +5883,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FFC5BD54-0ED4-2343-B851-95E8E334E765}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FFC5BD54-0ED4-2343-B851-95E8E334E765}" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A20:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField dataField="1" showAll="0"/>
@@ -5971,7 +5965,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4C07DF30-360B-9D4E-92AA-D9ACB16D7C47}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4C07DF30-360B-9D4E-92AA-D9ACB16D7C47}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField showAll="0"/>
@@ -6067,7 +6061,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{976BB6B3-7511-064E-88F6-64174885D19D}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{976BB6B3-7511-064E-88F6-64174885D19D}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A11:E17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="27">
     <pivotField showAll="0"/>
@@ -6168,37 +6162,43 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{310D2D95-3555-B746-82FE-2701FAF02A28}" name="Table3" displayName="Table3" ref="A1:AA93" totalsRowShown="0" dataDxfId="33">
-  <autoFilter ref="A1:AA93" xr:uid="{F5024BC6-9063-694A-A93E-42CCEC70DC0E}"/>
+  <autoFilter ref="A1:AA93" xr:uid="{F5024BC6-9063-694A-A93E-42CCEC70DC0E}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Traine"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{DF807125-8008-9B45-910F-BD5834AC4703}" name="Id " dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{DF807125-8008-9B45-910F-BD5834AC4703}" name="Id " dataDxfId="32">
       <calculatedColumnFormula>ROW(Table3[[#This Row],[Id ]])-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C9696508-EE25-1A45-B96C-08EAD40938A3}" name="Nom " dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{940E60E1-C7E1-4F4F-8895-E9FE0704C564}" name="Fonction " dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{C9696508-EE25-1A45-B96C-08EAD40938A3}" name="Nom " dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{940E60E1-C7E1-4F4F-8895-E9FE0704C564}" name="Fonction " dataDxfId="30"/>
     <tableColumn id="20" xr3:uid="{386A16F9-35AD-BB46-89D3-D9699EAC8FA7}" name="sex"/>
-    <tableColumn id="4" xr3:uid="{8E17B760-B8BE-864C-AF87-A9335C03E97C}" name="Position " dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{ABDCBFBF-B054-D146-B5E8-2CAEDF8514CC}" name="Description " dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{1B08239F-7E20-A64E-BC04-72A921E0E414}" name="Pouvoir_Actif " dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{F5E21B03-30F6-6741-8C09-CE41E1076FA1}" name="Pouvoir_Passif " dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{E2055E35-7F0B-6742-9A85-B10DCD92215A}" name="Tier " dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{5C51D725-F07A-6C4E-939F-1678E227FDBB}" name="Image " dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{C3E7EDE7-11C6-784D-87C7-D175E5B5DF38}" name="Extension" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{9940D91B-6F5F-404F-99B5-F72D8578A58B}" name="Noob" dataDxfId="23"/>
-    <tableColumn id="27" xr3:uid="{6CE36110-43AD-744A-9CC3-0E7ABFA50DCE}" name="Team" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{C1817EFB-B0DB-3F42-9A6F-F62A18CB30B8}" name="Team mixed" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{34D37E35-FFCB-4D41-A911-C0D18C6E8619}" name="Abandon" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{F5E0F745-61E7-354D-8680-94E0371B7A65}" name="Repos" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{EE8BD564-815F-524E-B24D-04B63C59C135}" name="Cumul de des" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{AA0F0E9F-DA18-834F-9E18-076EF0E20DA6}" name="Controle de des" dataDxfId="17"/>
-    <tableColumn id="17" xr3:uid="{E50864F6-A3F1-A642-ACA9-B70B42DC97C6}" name="Recrutement" dataDxfId="16"/>
-    <tableColumn id="18" xr3:uid="{5DDB2C9C-9E7A-1340-B637-B88A2371DD46}" name="Terrain" dataDxfId="15"/>
-    <tableColumn id="19" xr3:uid="{7EDCD20F-AF02-9347-BB90-A9D7EA3396EF}" name="Succes auto" dataDxfId="14"/>
-    <tableColumn id="21" xr3:uid="{D7B249E2-F696-BC41-9E15-A66CE8CF07A9}" name="Vent" dataDxfId="13"/>
-    <tableColumn id="22" xr3:uid="{93CCABF8-EEC0-CA4F-A19A-A636000739DC}" name="Autre" dataDxfId="12"/>
-    <tableColumn id="23" xr3:uid="{2E3A41D4-2BE3-594F-B2E8-5E80B13227D3}" name="Moral" dataDxfId="11"/>
-    <tableColumn id="24" xr3:uid="{77D877E7-6020-8D4C-8E2B-B7751C4CFDB8}" name="noir" dataDxfId="10"/>
-    <tableColumn id="25" xr3:uid="{5C9D01FD-00DD-E143-ACF5-35386360BB10}" name="conditionnel" dataDxfId="9"/>
-    <tableColumn id="26" xr3:uid="{43BF2869-DF4D-244E-A5E7-5A0AABCC8001}" name="range" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{8E17B760-B8BE-864C-AF87-A9335C03E97C}" name="Position " dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{ABDCBFBF-B054-D146-B5E8-2CAEDF8514CC}" name="Description " dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{1B08239F-7E20-A64E-BC04-72A921E0E414}" name="Pouvoir_Actif " dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{F5E21B03-30F6-6741-8C09-CE41E1076FA1}" name="Pouvoir_Passif " dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{E2055E35-7F0B-6742-9A85-B10DCD92215A}" name="Tier " dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{5C51D725-F07A-6C4E-939F-1678E227FDBB}" name="Image " dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{C3E7EDE7-11C6-784D-87C7-D175E5B5DF38}" name="Extension" dataDxfId="23"/>
+    <tableColumn id="16" xr3:uid="{9940D91B-6F5F-404F-99B5-F72D8578A58B}" name="Noob" dataDxfId="22"/>
+    <tableColumn id="27" xr3:uid="{6CE36110-43AD-744A-9CC3-0E7ABFA50DCE}" name="Team" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{C1817EFB-B0DB-3F42-9A6F-F62A18CB30B8}" name="Team mixed" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{34D37E35-FFCB-4D41-A911-C0D18C6E8619}" name="Abandon" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{F5E0F745-61E7-354D-8680-94E0371B7A65}" name="Repos" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{EE8BD564-815F-524E-B24D-04B63C59C135}" name="Cumul de des" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{AA0F0E9F-DA18-834F-9E18-076EF0E20DA6}" name="Controle de des" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{E50864F6-A3F1-A642-ACA9-B70B42DC97C6}" name="Recrutement" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{5DDB2C9C-9E7A-1340-B637-B88A2371DD46}" name="Terrain" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{7EDCD20F-AF02-9347-BB90-A9D7EA3396EF}" name="Succes auto" dataDxfId="13"/>
+    <tableColumn id="21" xr3:uid="{D7B249E2-F696-BC41-9E15-A66CE8CF07A9}" name="Vent" dataDxfId="12"/>
+    <tableColumn id="22" xr3:uid="{93CCABF8-EEC0-CA4F-A19A-A636000739DC}" name="Autre" dataDxfId="11"/>
+    <tableColumn id="23" xr3:uid="{2E3A41D4-2BE3-594F-B2E8-5E80B13227D3}" name="Moral" dataDxfId="10"/>
+    <tableColumn id="24" xr3:uid="{77D877E7-6020-8D4C-8E2B-B7751C4CFDB8}" name="noir" dataDxfId="9"/>
+    <tableColumn id="25" xr3:uid="{5C9D01FD-00DD-E143-ACF5-35386360BB10}" name="conditionnel" dataDxfId="8"/>
+    <tableColumn id="26" xr3:uid="{43BF2869-DF4D-244E-A5E7-5A0AABCC8001}" name="range" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6211,17 +6211,17 @@
     <sortCondition ref="B4:B96"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{15B79788-6A50-004A-9C65-5A7CE29E4E85}" name="nom" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{15B79788-6A50-004A-9C65-5A7CE29E4E85}" name="nom" dataDxfId="6">
       <calculatedColumnFormula>Data!B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{89CE6B9F-9DE4-7F4F-8DA3-134B104BF520}" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{3110C9A4-9AA8-EA4F-9AA5-B1392CD99116}" name="sex" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{89CE6B9F-9DE4-7F4F-8DA3-134B104BF520}" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{3110C9A4-9AA8-EA4F-9AA5-B1392CD99116}" name="sex" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[ID]],Table3[],4,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{C9A08096-FEC4-BD46-8050-415B8B94F40B}" name="Sexe" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{C9A08096-FEC4-BD46-8050-415B8B94F40B}" name="Sexe" dataDxfId="3">
       <calculatedColumnFormula>IF(Table1[[#This Row],[sex]]="man","homme","femme")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C4E2C68C-A8B8-B749-B066-E6C0C995F1ED}" name="description" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{C4E2C68C-A8B8-B749-B066-E6C0C995F1ED}" name="description" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[ID]],Table3[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{13C95F11-B306-694C-853A-A839038F6BC6}" name="caractere"/>
@@ -6248,7 +6248,7 @@
   <autoFilter ref="A1:B84" xr:uid="{0DC7CD4E-B000-2B42-B7F8-6D558D42A36C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{BE77A2C3-9258-274A-901E-31BC4218604C}" name="Portraits"/>
-    <tableColumn id="2" xr3:uid="{7B933783-DA5B-5841-9B15-A0E029DC782F}" name="Used" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{7B933783-DA5B-5841-9B15-A0E029DC782F}" name="Used" dataDxfId="0">
       <calculatedColumnFormula>VLOOKUP(portraits[[#This Row],[Portraits]],Table3[[Image ]],1,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6555,11 +6555,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4D1010-4D36-3C4D-9CF7-660420749DE7}">
   <dimension ref="A1:AA93"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J86" sqref="J86"/>
+      <selection pane="bottomRight" activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6576,7 +6576,8 @@
     <col min="10" max="10" width="30.1640625" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
     <col min="15" max="15" width="10.83203125" customWidth="1"/>
     <col min="16" max="16" width="8.6640625" customWidth="1"/>
     <col min="17" max="17" width="8.83203125" customWidth="1"/>
@@ -6672,7 +6673,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>1</v>
@@ -6720,7 +6721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>2</v>
@@ -6768,7 +6769,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>3</v>
@@ -6810,7 +6811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>4</v>
@@ -6858,7 +6859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>5</v>
@@ -6906,7 +6907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>6</v>
@@ -6954,7 +6955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>7</v>
@@ -7005,7 +7006,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>8</v>
@@ -7050,7 +7051,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>9</v>
@@ -7098,7 +7099,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>10</v>
@@ -7149,7 +7150,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>11</v>
@@ -7197,7 +7198,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>12</v>
@@ -7248,7 +7249,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>13</v>
@@ -7302,7 +7303,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>14</v>
@@ -7350,7 +7351,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>15</v>
@@ -7401,7 +7402,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>16</v>
@@ -7455,7 +7456,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>17</v>
@@ -7506,7 +7507,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>18</v>
@@ -7560,7 +7561,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>19</v>
@@ -7611,7 +7612,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>20</v>
@@ -7662,7 +7663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>21</v>
@@ -7713,7 +7714,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>22</v>
@@ -7764,7 +7765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>23</v>
@@ -7818,7 +7819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>24</v>
@@ -7869,7 +7870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>25</v>
@@ -7917,7 +7918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>26</v>
@@ -7968,7 +7969,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>27</v>
@@ -8016,7 +8017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>28</v>
@@ -8061,7 +8062,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>29</v>
@@ -8115,7 +8116,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>30</v>
@@ -8166,7 +8167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>31</v>
@@ -8220,7 +8221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>32</v>
@@ -8271,7 +8272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>33</v>
@@ -8322,7 +8323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>34</v>
@@ -8373,7 +8374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>35</v>
@@ -8415,7 +8416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>36</v>
@@ -8706,7 +8707,7 @@
         <v>677</v>
       </c>
       <c r="M43" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="N43" t="s">
         <v>423</v>
@@ -8750,6 +8751,9 @@
       <c r="J44" t="s">
         <v>76</v>
       </c>
+      <c r="M44" t="s">
+        <v>423</v>
+      </c>
       <c r="N44" t="s">
         <v>402</v>
       </c>
@@ -8792,9 +8796,6 @@
       <c r="J45" t="s">
         <v>60</v>
       </c>
-      <c r="M45" t="s">
-        <v>426</v>
-      </c>
       <c r="N45" t="s">
         <v>426</v>
       </c>
@@ -8834,6 +8835,9 @@
       <c r="J46" t="s">
         <v>699</v>
       </c>
+      <c r="M46" t="s">
+        <v>404</v>
+      </c>
       <c r="N46" t="s">
         <v>403</v>
       </c>
@@ -8960,9 +8964,6 @@
       <c r="J49" t="s">
         <v>569</v>
       </c>
-      <c r="M49" t="s">
-        <v>404</v>
-      </c>
       <c r="N49" t="s">
         <v>404</v>
       </c>
@@ -9237,7 +9238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>55</v>
@@ -9279,7 +9280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>56</v>
@@ -9321,7 +9322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>57</v>
@@ -9363,7 +9364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>58</v>
@@ -9411,7 +9412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>59</v>
@@ -9459,7 +9460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>60</v>
@@ -9510,7 +9511,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>61</v>
@@ -9561,7 +9562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>62</v>
@@ -9609,7 +9610,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>63</v>
@@ -9657,7 +9658,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>64</v>
@@ -9705,7 +9706,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>65</v>
@@ -9759,7 +9760,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>66</v>
@@ -9807,7 +9808,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>67</v>
@@ -9855,7 +9856,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>68</v>
@@ -9903,7 +9904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>69</v>
@@ -9951,7 +9952,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>70</v>
@@ -9996,7 +9997,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>71</v>
@@ -10050,7 +10051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>72</v>
@@ -10112,7 +10113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>73</v>
@@ -10160,7 +10161,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>74</v>
@@ -10525,7 +10526,7 @@
       <c r="I83">
         <v>2</v>
       </c>
-      <c r="J83" s="11" t="s">
+      <c r="J83" t="s">
         <v>900</v>
       </c>
       <c r="K83" t="s">
@@ -10720,305 +10721,203 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>87</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" t="s">
         <v>809</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" t="s">
         <v>1</v>
       </c>
       <c r="D88" t="s">
         <v>470</v>
       </c>
-      <c r="E88" s="8" t="s">
+      <c r="E88" t="s">
         <v>2</v>
       </c>
-      <c r="F88" s="8" t="s">
+      <c r="F88" t="s">
         <v>816</v>
       </c>
-      <c r="G88" s="8" t="s">
+      <c r="G88" t="s">
         <v>810</v>
       </c>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8">
+      <c r="I88">
         <v>3</v>
       </c>
-      <c r="J88" s="8" t="s">
+      <c r="J88" t="s">
         <v>817</v>
       </c>
       <c r="K88" t="s">
         <v>218</v>
       </c>
-      <c r="L88" s="8"/>
-      <c r="M88" s="8"/>
-      <c r="N88" s="8"/>
-      <c r="O88" s="8"/>
-      <c r="P88" s="8"/>
-      <c r="Q88" s="8"/>
-      <c r="R88" s="8"/>
-      <c r="S88" s="8"/>
-      <c r="T88" s="8"/>
-      <c r="U88" s="8"/>
-      <c r="V88" s="8"/>
-      <c r="W88" s="8"/>
-      <c r="X88" s="8"/>
-      <c r="Y88" s="8"/>
-      <c r="Z88" s="8"/>
-      <c r="AA88" s="8"/>
-    </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>88</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" t="s">
         <v>814</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C89" t="s">
         <v>824</v>
       </c>
       <c r="D89" t="s">
         <v>471</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E89" t="s">
         <v>7</v>
       </c>
-      <c r="F89" s="8" t="s">
+      <c r="F89" t="s">
         <v>818</v>
       </c>
-      <c r="G89" s="8" t="s">
+      <c r="G89" t="s">
         <v>841</v>
       </c>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8">
-        <v>1</v>
-      </c>
-      <c r="J89" s="8" t="s">
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="J89" t="s">
         <v>823</v>
       </c>
       <c r="K89" t="s">
         <v>218</v>
       </c>
-      <c r="L89" s="8"/>
-      <c r="M89" s="8"/>
-      <c r="N89" s="8"/>
-      <c r="O89" s="8"/>
-      <c r="P89" s="8"/>
-      <c r="Q89" s="8"/>
-      <c r="R89" s="8"/>
-      <c r="S89" s="8"/>
-      <c r="T89" s="8"/>
-      <c r="U89" s="8"/>
-      <c r="V89" s="8"/>
-      <c r="W89" s="8"/>
-      <c r="X89" s="8"/>
-      <c r="Y89" s="8"/>
-      <c r="Z89" s="8"/>
-      <c r="AA89" s="8"/>
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A90">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>89</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B90" t="s">
         <v>815</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C90" t="s">
         <v>61</v>
       </c>
       <c r="D90" t="s">
         <v>470</v>
       </c>
-      <c r="E90" s="8" t="s">
+      <c r="E90" t="s">
         <v>50</v>
       </c>
-      <c r="F90" s="8" t="s">
+      <c r="F90" t="s">
         <v>825</v>
       </c>
-      <c r="G90" s="8" t="s">
+      <c r="G90" t="s">
         <v>831</v>
       </c>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8">
+      <c r="I90">
         <v>2</v>
       </c>
-      <c r="J90" s="8" t="s">
+      <c r="J90" t="s">
         <v>830</v>
       </c>
       <c r="K90" t="s">
         <v>218</v>
       </c>
-      <c r="L90" s="8"/>
-      <c r="M90" s="8"/>
-      <c r="N90" s="8"/>
-      <c r="O90" s="8"/>
-      <c r="P90" s="8"/>
-      <c r="Q90" s="8"/>
-      <c r="R90" s="8"/>
-      <c r="S90" s="8"/>
-      <c r="T90" s="8"/>
-      <c r="U90" s="8"/>
-      <c r="V90" s="8"/>
-      <c r="W90" s="8"/>
-      <c r="X90" s="8"/>
-      <c r="Y90" s="8"/>
-      <c r="Z90" s="8"/>
-      <c r="AA90" s="8"/>
-    </row>
-    <row r="91" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:27" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>90</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" t="s">
         <v>832</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C91" t="s">
         <v>833</v>
       </c>
       <c r="D91" t="s">
         <v>470</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="E91" t="s">
         <v>23</v>
       </c>
-      <c r="F91" s="8" t="s">
+      <c r="F91" t="s">
         <v>834</v>
       </c>
-      <c r="G91" s="10" t="s">
+      <c r="G91" s="7" t="s">
         <v>878</v>
       </c>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8">
+      <c r="I91">
         <v>2</v>
       </c>
-      <c r="J91" s="8" t="s">
+      <c r="J91" t="s">
         <v>835</v>
       </c>
       <c r="K91" t="s">
         <v>218</v>
       </c>
-      <c r="L91" s="8"/>
-      <c r="M91" s="8"/>
-      <c r="N91" s="8"/>
-      <c r="O91" s="8"/>
-      <c r="P91" s="8"/>
-      <c r="Q91" s="8"/>
-      <c r="R91" s="8"/>
-      <c r="S91" s="8"/>
-      <c r="T91" s="8"/>
-      <c r="U91" s="8"/>
-      <c r="V91" s="8"/>
-      <c r="W91" s="8"/>
-      <c r="X91" s="8"/>
-      <c r="Y91" s="8"/>
-      <c r="Z91" s="8"/>
-      <c r="AA91" s="8"/>
-    </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>91</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" t="s">
         <v>858</v>
       </c>
-      <c r="C92" s="8" t="s">
+      <c r="C92" t="s">
         <v>856</v>
       </c>
       <c r="D92" t="s">
         <v>856</v>
       </c>
-      <c r="E92" s="8" t="s">
+      <c r="E92" t="s">
         <v>23</v>
       </c>
-      <c r="F92" s="8" t="s">
+      <c r="F92" t="s">
         <v>864</v>
       </c>
-      <c r="G92" s="8" t="s">
+      <c r="G92" t="s">
         <v>865</v>
       </c>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8">
-        <v>1</v>
-      </c>
-      <c r="J92" s="8" t="s">
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92" t="s">
         <v>866</v>
       </c>
       <c r="K92" t="s">
         <v>218</v>
       </c>
-      <c r="L92" s="8"/>
-      <c r="M92" s="8"/>
-      <c r="N92" s="8"/>
-      <c r="O92" s="8"/>
-      <c r="P92" s="8"/>
-      <c r="Q92" s="8"/>
-      <c r="R92" s="8"/>
-      <c r="S92" s="8"/>
-      <c r="T92" s="8"/>
-      <c r="U92" s="8"/>
-      <c r="V92" s="8"/>
-      <c r="W92" s="8"/>
-      <c r="X92" s="8"/>
-      <c r="Y92" s="8"/>
-      <c r="Z92" s="8"/>
-      <c r="AA92" s="8"/>
     </row>
     <row r="93" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A93">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>92</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="B93" t="s">
         <v>860</v>
       </c>
-      <c r="C93" s="8" t="s">
+      <c r="C93" t="s">
         <v>859</v>
       </c>
       <c r="D93" t="s">
         <v>471</v>
       </c>
-      <c r="E93" s="8" t="s">
+      <c r="E93" t="s">
         <v>50</v>
       </c>
-      <c r="F93" s="8" t="s">
+      <c r="F93" t="s">
         <v>868</v>
       </c>
-      <c r="G93" s="10" t="s">
+      <c r="G93" s="7" t="s">
         <v>877</v>
       </c>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8">
+      <c r="I93">
         <v>2</v>
       </c>
-      <c r="J93" s="8" t="s">
+      <c r="J93" t="s">
         <v>867</v>
       </c>
       <c r="K93" t="s">
         <v>218</v>
       </c>
-      <c r="L93" s="8"/>
-      <c r="M93" s="8"/>
-      <c r="N93" s="8"/>
-      <c r="O93" s="8"/>
-      <c r="P93" s="8"/>
-      <c r="Q93" s="8"/>
-      <c r="R93" s="8"/>
-      <c r="S93" s="8"/>
-      <c r="T93" s="8"/>
-      <c r="U93" s="8"/>
-      <c r="V93" s="8"/>
-      <c r="W93" s="8"/>
-      <c r="X93" s="8"/>
-      <c r="Y93" s="8"/>
-      <c r="Z93" s="8"/>
-      <c r="AA93" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11036,7 +10935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35366886-6F09-7944-A368-692B97213087}">
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -11123,7 +11022,7 @@
       <c r="I5" t="s">
         <v>486</v>
       </c>
-      <c r="J5" s="11" t="str">
+      <c r="J5" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11174,7 +11073,7 @@
       <c r="I6" t="s">
         <v>487</v>
       </c>
-      <c r="J6" s="11" t="str">
+      <c r="J6" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11225,7 +11124,7 @@
       <c r="I7" t="s">
         <v>490</v>
       </c>
-      <c r="J7" s="11" t="str">
+      <c r="J7" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11276,7 +11175,7 @@
       <c r="I8" t="s">
         <v>727</v>
       </c>
-      <c r="J8" s="11" t="str">
+      <c r="J8" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11327,7 +11226,7 @@
       <c r="I9" t="s">
         <v>728</v>
       </c>
-      <c r="J9" s="11" t="str">
+      <c r="J9" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11378,7 +11277,7 @@
       <c r="I10" t="s">
         <v>500</v>
       </c>
-      <c r="J10" s="11" t="str">
+      <c r="J10" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11429,7 +11328,7 @@
       <c r="I11" t="s">
         <v>500</v>
       </c>
-      <c r="J11" s="11" t="str">
+      <c r="J11" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11480,7 +11379,7 @@
       <c r="I12" t="s">
         <v>505</v>
       </c>
-      <c r="J12" s="11" t="str">
+      <c r="J12" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11531,7 +11430,7 @@
       <c r="I13" t="s">
         <v>512</v>
       </c>
-      <c r="J13" s="11" t="str">
+      <c r="J13" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11582,7 +11481,7 @@
       <c r="I14" t="s">
         <v>513</v>
       </c>
-      <c r="J14" s="11" t="str">
+      <c r="J14" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11633,7 +11532,7 @@
       <c r="I15" t="s">
         <v>524</v>
       </c>
-      <c r="J15" s="11" t="str">
+      <c r="J15" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11684,7 +11583,7 @@
       <c r="I16" t="s">
         <v>528</v>
       </c>
-      <c r="J16" s="11" t="str">
+      <c r="J16" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11735,7 +11634,7 @@
       <c r="I17" t="s">
         <v>530</v>
       </c>
-      <c r="J17" s="11" t="str">
+      <c r="J17" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11786,7 +11685,7 @@
       <c r="I18" t="s">
         <v>536</v>
       </c>
-      <c r="J18" s="11" t="str">
+      <c r="J18" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11837,7 +11736,7 @@
       <c r="I19" t="s">
         <v>546</v>
       </c>
-      <c r="J19" s="11" t="str">
+      <c r="J19" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11888,7 +11787,7 @@
       <c r="I20" t="s">
         <v>555</v>
       </c>
-      <c r="J20" s="11" t="str">
+      <c r="J20" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11939,7 +11838,7 @@
       <c r="I21" t="s">
         <v>551</v>
       </c>
-      <c r="J21" s="11" t="str">
+      <c r="J21" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -11990,7 +11889,7 @@
       <c r="I22" t="s">
         <v>561</v>
       </c>
-      <c r="J22" s="11" t="str">
+      <c r="J22" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12041,7 +11940,7 @@
       <c r="I23" t="s">
         <v>563</v>
       </c>
-      <c r="J23" s="11" t="str">
+      <c r="J23" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12092,7 +11991,7 @@
       <c r="I24" t="s">
         <v>568</v>
       </c>
-      <c r="J24" s="11" t="str">
+      <c r="J24" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12143,7 +12042,7 @@
       <c r="I25" t="s">
         <v>573</v>
       </c>
-      <c r="J25" s="11" t="str">
+      <c r="J25" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12194,7 +12093,7 @@
       <c r="I26" t="s">
         <v>573</v>
       </c>
-      <c r="J26" s="11" t="str">
+      <c r="J26" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12245,7 +12144,7 @@
       <c r="I27" t="s">
         <v>576</v>
       </c>
-      <c r="J27" s="11" t="str">
+      <c r="J27" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12296,7 +12195,7 @@
       <c r="I28" t="s">
         <v>576</v>
       </c>
-      <c r="J28" s="11" t="str">
+      <c r="J28" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12347,7 +12246,7 @@
       <c r="I29" t="s">
         <v>582</v>
       </c>
-      <c r="J29" s="11" t="str">
+      <c r="J29" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12398,7 +12297,7 @@
       <c r="I30" t="s">
         <v>586</v>
       </c>
-      <c r="J30" s="11" t="str">
+      <c r="J30" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12449,7 +12348,7 @@
       <c r="I31" t="s">
         <v>596</v>
       </c>
-      <c r="J31" s="11" t="str">
+      <c r="J31" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12500,7 +12399,7 @@
       <c r="I32" t="s">
         <v>602</v>
       </c>
-      <c r="J32" s="11" t="str">
+      <c r="J32" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12551,7 +12450,7 @@
       <c r="I33" t="s">
         <v>608</v>
       </c>
-      <c r="J33" s="11" t="str">
+      <c r="J33" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12602,7 +12501,7 @@
       <c r="I34" t="s">
         <v>611</v>
       </c>
-      <c r="J34" s="11" t="str">
+      <c r="J34" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12653,7 +12552,7 @@
       <c r="I35" t="s">
         <v>616</v>
       </c>
-      <c r="J35" s="11" t="str">
+      <c r="J35" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12704,7 +12603,7 @@
       <c r="I36" t="s">
         <v>620</v>
       </c>
-      <c r="J36" s="11" t="str">
+      <c r="J36" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12755,7 +12654,7 @@
       <c r="I37" t="s">
         <v>626</v>
       </c>
-      <c r="J37" s="11" t="str">
+      <c r="J37" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12794,7 +12693,7 @@
         <f>VLOOKUP(Table1[[#This Row],[ID]],Table3[],6,FALSE)</f>
         <v xml:space="preserve">Le vent souffle dans l'oreille de Wanda et Wanda souffle a l'oreille du traceur. </v>
       </c>
-      <c r="J38" s="11" t="str">
+      <c r="J38" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12845,7 +12744,7 @@
       <c r="I39" t="s">
         <v>629</v>
       </c>
-      <c r="J39" s="11" t="str">
+      <c r="J39" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12896,7 +12795,7 @@
       <c r="I40" t="s">
         <v>634</v>
       </c>
-      <c r="J40" s="11" t="str">
+      <c r="J40" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12943,7 +12842,7 @@
       <c r="H41" t="s">
         <v>635</v>
       </c>
-      <c r="J41" s="11" t="str">
+      <c r="J41" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -12990,7 +12889,7 @@
       <c r="H42" t="s">
         <v>640</v>
       </c>
-      <c r="J42" s="11" t="str">
+      <c r="J42" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13041,7 +12940,7 @@
       <c r="I43" t="s">
         <v>648</v>
       </c>
-      <c r="J43" s="11" t="str">
+      <c r="J43" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13092,7 +12991,7 @@
       <c r="I44" t="s">
         <v>653</v>
       </c>
-      <c r="J44" s="11" t="str">
+      <c r="J44" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13143,7 +13042,7 @@
       <c r="I45" t="s">
         <v>657</v>
       </c>
-      <c r="J45" s="11" t="str">
+      <c r="J45" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13194,7 +13093,7 @@
       <c r="I46" t="s">
         <v>664</v>
       </c>
-      <c r="J46" s="11" t="str">
+      <c r="J46" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13245,7 +13144,7 @@
       <c r="I47" t="s">
         <v>670</v>
       </c>
-      <c r="J47" s="11" t="str">
+      <c r="J47" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13293,7 +13192,7 @@
       <c r="I48" t="s">
         <v>673</v>
       </c>
-      <c r="J48" s="11" t="str">
+      <c r="J48" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13344,7 +13243,7 @@
       <c r="I49" t="s">
         <v>691</v>
       </c>
-      <c r="J49" s="11" t="str">
+      <c r="J49" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13395,7 +13294,7 @@
       <c r="I50" t="s">
         <v>648</v>
       </c>
-      <c r="J50" s="11" t="str">
+      <c r="J50" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13443,7 +13342,7 @@
       <c r="I51" t="s">
         <v>673</v>
       </c>
-      <c r="J51" s="11" t="str">
+      <c r="J51" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13494,7 +13393,7 @@
       <c r="I52" t="s">
         <v>543</v>
       </c>
-      <c r="J52" s="11" t="str">
+      <c r="J52" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13545,7 +13444,7 @@
       <c r="I53" t="s">
         <v>684</v>
       </c>
-      <c r="J53" s="11" t="str">
+      <c r="J53" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13596,7 +13495,7 @@
       <c r="I54" t="s">
         <v>698</v>
       </c>
-      <c r="J54" s="11" t="str">
+      <c r="J54" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13647,7 +13546,7 @@
       <c r="I55" t="s">
         <v>676</v>
       </c>
-      <c r="J55" s="11" t="str">
+      <c r="J55" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13698,7 +13597,7 @@
       <c r="I56" t="s">
         <v>682</v>
       </c>
-      <c r="J56" s="11" t="str">
+      <c r="J56" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13749,7 +13648,7 @@
       <c r="I57" t="s">
         <v>706</v>
       </c>
-      <c r="J57" s="11" t="str">
+      <c r="J57" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13800,7 +13699,7 @@
       <c r="I58" t="s">
         <v>714</v>
       </c>
-      <c r="J58" s="11" t="str">
+      <c r="J58" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13851,7 +13750,7 @@
       <c r="I59" t="s">
         <v>713</v>
       </c>
-      <c r="J59" s="11" t="str">
+      <c r="J59" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13902,7 +13801,7 @@
       <c r="I60" t="s">
         <v>716</v>
       </c>
-      <c r="J60" s="11" t="str">
+      <c r="J60" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -13953,7 +13852,7 @@
       <c r="I61" t="s">
         <v>731</v>
       </c>
-      <c r="J61" s="11" t="str">
+      <c r="J61" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14004,7 +13903,7 @@
       <c r="I62" t="s">
         <v>733</v>
       </c>
-      <c r="J62" s="11" t="str">
+      <c r="J62" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14055,7 +13954,7 @@
       <c r="I63" t="s">
         <v>737</v>
       </c>
-      <c r="J63" s="11" t="str">
+      <c r="J63" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14106,7 +14005,7 @@
       <c r="I64" t="s">
         <v>741</v>
       </c>
-      <c r="J64" s="11" t="str">
+      <c r="J64" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14157,7 +14056,7 @@
       <c r="I65" t="s">
         <v>746</v>
       </c>
-      <c r="J65" s="11" t="str">
+      <c r="J65" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14208,7 +14107,7 @@
       <c r="I66" t="s">
         <v>749</v>
       </c>
-      <c r="J66" s="11" t="str">
+      <c r="J66" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14259,7 +14158,7 @@
       <c r="I67" t="s">
         <v>500</v>
       </c>
-      <c r="J67" s="11" t="str">
+      <c r="J67" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14310,7 +14209,7 @@
       <c r="I68" t="s">
         <v>750</v>
       </c>
-      <c r="J68" s="11" t="str">
+      <c r="J68" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14361,7 +14260,7 @@
       <c r="I69" t="s">
         <v>755</v>
       </c>
-      <c r="J69" s="11" t="str">
+      <c r="J69" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14412,7 +14311,7 @@
       <c r="I70" t="s">
         <v>763</v>
       </c>
-      <c r="J70" s="11" t="str">
+      <c r="J70" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14463,7 +14362,7 @@
       <c r="I71" t="s">
         <v>775</v>
       </c>
-      <c r="J71" s="11" t="str">
+      <c r="J71" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14514,7 +14413,7 @@
       <c r="I72" t="s">
         <v>778</v>
       </c>
-      <c r="J72" s="11" t="str">
+      <c r="J72" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14565,7 +14464,7 @@
       <c r="I73" t="s">
         <v>784</v>
       </c>
-      <c r="J73" s="11" t="str">
+      <c r="J73" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14616,7 +14515,7 @@
       <c r="I74" t="s">
         <v>786</v>
       </c>
-      <c r="J74" s="11" t="str">
+      <c r="J74" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14655,7 +14554,7 @@
         <f>VLOOKUP(Table1[[#This Row],[ID]],Table3[],6,FALSE)</f>
         <v xml:space="preserve">Les frères Torantor sont des valeurs sûres. Solides sur leurs appuis ils renforcent le groupe avec bienveillance. </v>
       </c>
-      <c r="J75" s="11" t="str">
+      <c r="J75" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14706,7 +14605,7 @@
       <c r="I76" t="s">
         <v>495</v>
       </c>
-      <c r="J76" s="11" t="str">
+      <c r="J76" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14757,7 +14656,7 @@
       <c r="I77" t="s">
         <v>793</v>
       </c>
-      <c r="J77" s="11" t="str">
+      <c r="J77" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14808,7 +14707,7 @@
       <c r="I78" t="s">
         <v>798</v>
       </c>
-      <c r="J78" s="11" t="str">
+      <c r="J78" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14859,7 +14758,7 @@
       <c r="I79" t="s">
         <v>802</v>
       </c>
-      <c r="J79" s="11" t="str">
+      <c r="J79" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14901,7 +14800,7 @@
       <c r="F80" t="s">
         <v>801</v>
       </c>
-      <c r="J80" s="11" t="str">
+      <c r="J80" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14946,7 +14845,7 @@
       <c r="I81" t="s">
         <v>805</v>
       </c>
-      <c r="J81" s="11" t="str">
+      <c r="J81" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -14988,7 +14887,7 @@
       <c r="I82" t="s">
         <v>702</v>
       </c>
-      <c r="J82" s="11" t="str">
+      <c r="J82" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15033,7 +14932,7 @@
       <c r="I83" t="s">
         <v>807</v>
       </c>
-      <c r="J83" s="11" t="str">
+      <c r="J83" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15084,7 +14983,7 @@
       <c r="I84" t="s">
         <v>848</v>
       </c>
-      <c r="J84" s="11" t="str">
+      <c r="J84" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15135,7 +15034,7 @@
       <c r="I85" t="s">
         <v>852</v>
       </c>
-      <c r="J85" s="11" t="str">
+      <c r="J85" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15186,7 +15085,7 @@
       <c r="I86" t="s">
         <v>896</v>
       </c>
-      <c r="J86" s="11" t="str">
+      <c r="J86" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15237,7 +15136,7 @@
       <c r="I87" t="s">
         <v>890</v>
       </c>
-      <c r="J87" s="11" t="str">
+      <c r="J87" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15288,7 +15187,7 @@
       <c r="I88" t="s">
         <v>880</v>
       </c>
-      <c r="J88" s="11" t="str">
+      <c r="J88" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15339,7 +15238,7 @@
       <c r="I89" t="s">
         <v>870</v>
       </c>
-      <c r="J89" s="11" t="str">
+      <c r="J89" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15378,7 +15277,7 @@
         <f>VLOOKUP(Table1[[#This Row],[ID]],Table3[],6,FALSE)</f>
         <v xml:space="preserve">Les frères Torantor sont des valeurs sûres. Solides sur leurs appuis ils renforcent le groupe avec bienveillance. </v>
       </c>
-      <c r="J90" s="11" t="str">
+      <c r="J90" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15429,7 +15328,7 @@
       <c r="I91" t="s">
         <v>813</v>
       </c>
-      <c r="J91" s="11" t="str">
+      <c r="J91" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15551,22 +15450,22 @@
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" s="9" t="str">
+      <c r="A94" t="str">
         <f>Data!B91</f>
         <v>Le Daron</v>
       </c>
-      <c r="B94" s="9">
+      <c r="B94">
         <v>90</v>
       </c>
-      <c r="C94" s="9" t="str">
+      <c r="C94" t="str">
         <f>VLOOKUP(Table1[[#This Row],[ID]],Table3[],4,FALSE)</f>
         <v>man</v>
       </c>
-      <c r="D94" s="9" t="str">
+      <c r="D94" t="str">
         <f>IF(Table1[[#This Row],[sex]]="man","homme","femme")</f>
         <v>homme</v>
       </c>
-      <c r="E94" s="9" t="str">
+      <c r="E94" t="str">
         <f>VLOOKUP(Table1[[#This Row],[ID]],Table3[],6,FALSE)</f>
         <v>Le Daron s'occupe de l'equipe, nettoye et range vite le materiel en bordel mais mal…</v>
       </c>
@@ -15582,7 +15481,7 @@
       <c r="I94" t="s">
         <v>840</v>
       </c>
-      <c r="J94" s="9" t="str">
+      <c r="J94" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15602,22 +15501,22 @@
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A95" s="9" t="str">
+      <c r="A95" t="str">
         <f>Data!B92</f>
         <v>Le Dragon</v>
       </c>
-      <c r="B95" s="9">
+      <c r="B95">
         <v>91</v>
       </c>
-      <c r="C95" s="9" t="str">
+      <c r="C95" t="str">
         <f>VLOOKUP(Table1[[#This Row],[ID]],Table3[],4,FALSE)</f>
         <v>dragon</v>
       </c>
-      <c r="D95" s="9" t="str">
+      <c r="D95" t="str">
         <f>IF(Table1[[#This Row],[sex]]="man","homme","femme")</f>
         <v>femme</v>
       </c>
-      <c r="E95" s="9" t="str">
+      <c r="E95" t="str">
         <f>VLOOKUP(Table1[[#This Row],[ID]],Table3[],6,FALSE)</f>
         <v xml:space="preserve">Le Dragon </v>
       </c>
@@ -15633,7 +15532,7 @@
       <c r="I95" t="s">
         <v>857</v>
       </c>
-      <c r="J95" s="9" t="str">
+      <c r="J95" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -15653,22 +15552,21 @@
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" s="9" t="str">
+      <c r="A96" t="str">
         <f>Data!B93</f>
         <v>Unicorn</v>
       </c>
-      <c r="B96" s="9">
+      <c r="B96">
         <v>92</v>
       </c>
-      <c r="C96" s="9" t="str">
+      <c r="C96" t="str">
         <f>VLOOKUP(Table1[[#This Row],[ID]],Table3[],4,FALSE)</f>
         <v>woman</v>
       </c>
-      <c r="D96" s="9" t="str">
+      <c r="D96" t="str">
         <f>IF(Table1[[#This Row],[sex]]="man","homme","femme")</f>
         <v>femme</v>
       </c>
-      <c r="E96" s="9"/>
       <c r="F96" t="s">
         <v>861</v>
       </c>
@@ -15681,7 +15579,7 @@
       <c r="I96" t="s">
         <v>822</v>
       </c>
-      <c r="J96" s="9" t="str">
+      <c r="J96" t="str">
         <f>_xlfn.CONCAT("Personnage ",Table1[[#This Row],[ID]],"
 style de dessin: Esquisse au crayon de papier réaliste, portrait seulement, fond blanc, medieval fantastic, steampunk
 Caractère : ",Table1[[#This Row],[caractere]],"
@@ -16673,13 +16571,13 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5">
         <v>8</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5">
         <v>13</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5">
         <v>21</v>
       </c>
     </row>
@@ -16687,13 +16585,13 @@
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
         <v>11</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6">
         <v>18</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6">
         <v>29</v>
       </c>
     </row>
@@ -16701,13 +16599,13 @@
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7">
         <v>10</v>
       </c>
     </row>
@@ -16715,13 +16613,13 @@
       <c r="A8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8">
         <v>14</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8">
         <v>18</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8">
         <v>32</v>
       </c>
     </row>
@@ -16729,13 +16627,13 @@
       <c r="A9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9">
         <v>38</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9">
         <v>54</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9">
         <v>92</v>
       </c>
     </row>
@@ -16768,16 +16666,16 @@
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13">
         <v>6</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13">
         <v>9</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13">
         <v>21</v>
       </c>
     </row>
@@ -16785,16 +16683,16 @@
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14">
         <v>15</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14">
         <v>9</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14">
         <v>5</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14">
         <v>29</v>
       </c>
     </row>
@@ -16802,16 +16700,16 @@
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15">
         <v>3</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15">
         <v>10</v>
       </c>
     </row>
@@ -16819,16 +16717,16 @@
       <c r="A16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16">
         <v>9</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16">
         <v>14</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16">
         <v>9</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16">
         <v>32</v>
       </c>
     </row>
@@ -16836,16 +16734,16 @@
       <c r="A17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17">
         <v>34</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17">
         <v>32</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17">
         <v>26</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17">
         <v>92</v>
       </c>
     </row>
@@ -16861,7 +16759,7 @@
       <c r="A21" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21">
         <v>1</v>
       </c>
     </row>
@@ -16869,7 +16767,7 @@
       <c r="A22" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22">
         <v>1</v>
       </c>
     </row>
@@ -16877,7 +16775,7 @@
       <c r="A23" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23">
         <v>1</v>
       </c>
     </row>
@@ -16885,7 +16783,7 @@
       <c r="A24" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24">
         <v>51</v>
       </c>
     </row>
@@ -16893,7 +16791,7 @@
       <c r="A25" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25">
         <v>38</v>
       </c>
     </row>
@@ -16901,7 +16799,7 @@
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nouvelle icone moral, plus gros des
</commit_message>
<xml_diff>
--- a/src/resources/horde_cards.xlsx
+++ b/src/resources/horde_cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsaban/git/perso/windwalkers-cardgame/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC85CA59-4782-2140-BA22-C2E9E182004D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA198F0D-64D4-014E-B382-B8B0238151FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="1280" windowWidth="27540" windowHeight="15340" xr2:uid="{2F94C834-2D3B-4040-A9EF-5D9A64AD9988}"/>
   </bookViews>
@@ -6162,13 +6162,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{310D2D95-3555-B746-82FE-2701FAF02A28}" name="Table3" displayName="Table3" ref="A1:AA93" totalsRowShown="0" dataDxfId="33">
-  <autoFilter ref="A1:AA93" xr:uid="{F5024BC6-9063-694A-A93E-42CCEC70DC0E}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Traine"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AA93" xr:uid="{F5024BC6-9063-694A-A93E-42CCEC70DC0E}"/>
   <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{DF807125-8008-9B45-910F-BD5834AC4703}" name="Id " dataDxfId="32">
       <calculatedColumnFormula>ROW(Table3[[#This Row],[Id ]])-1</calculatedColumnFormula>
@@ -6556,10 +6550,10 @@
   <dimension ref="A1:AA93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J41" sqref="J41"/>
+      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6673,7 +6667,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>1</v>
@@ -6721,7 +6715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>2</v>
@@ -6769,7 +6763,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>3</v>
@@ -6811,7 +6805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>4</v>
@@ -6859,7 +6853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>5</v>
@@ -6907,7 +6901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>6</v>
@@ -6955,7 +6949,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>7</v>
@@ -7006,7 +7000,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>8</v>
@@ -7051,7 +7045,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>9</v>
@@ -7099,7 +7093,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>10</v>
@@ -7150,7 +7144,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>11</v>
@@ -7198,7 +7192,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>12</v>
@@ -7249,7 +7243,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>13</v>
@@ -7303,7 +7297,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>14</v>
@@ -7351,7 +7345,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>15</v>
@@ -7402,7 +7396,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>16</v>
@@ -7456,7 +7450,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="18" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>17</v>
@@ -7507,7 +7501,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="19" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>18</v>
@@ -7561,7 +7555,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="20" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>19</v>
@@ -7612,7 +7606,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>20</v>
@@ -7663,7 +7657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>21</v>
@@ -7714,7 +7708,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>22</v>
@@ -7765,7 +7759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>23</v>
@@ -7819,7 +7813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>24</v>
@@ -7870,7 +7864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>25</v>
@@ -7918,7 +7912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>26</v>
@@ -7969,7 +7963,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="28" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>27</v>
@@ -8017,7 +8011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>28</v>
@@ -8062,7 +8056,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="30" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>29</v>
@@ -8116,7 +8110,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>30</v>
@@ -8167,7 +8161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>31</v>
@@ -8221,7 +8215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>32</v>
@@ -8272,7 +8266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>33</v>
@@ -8323,7 +8317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>34</v>
@@ -8374,7 +8368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>35</v>
@@ -8416,7 +8410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>36</v>
@@ -8577,6 +8571,9 @@
       <c r="L40" t="s">
         <v>404</v>
       </c>
+      <c r="M40" t="s">
+        <v>404</v>
+      </c>
       <c r="N40" t="s">
         <v>402</v>
       </c>
@@ -9006,9 +9003,6 @@
       <c r="J50" t="s">
         <v>687</v>
       </c>
-      <c r="M50" t="s">
-        <v>404</v>
-      </c>
       <c r="N50" t="s">
         <v>404</v>
       </c>
@@ -9238,7 +9232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A56">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>55</v>
@@ -9280,7 +9274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A57">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>56</v>
@@ -9322,7 +9316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A58">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>57</v>
@@ -9364,7 +9358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A59">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>58</v>
@@ -9412,7 +9406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A60">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>59</v>
@@ -9460,7 +9454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A61">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>60</v>
@@ -9511,7 +9505,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="62" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A62">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>61</v>
@@ -9562,7 +9556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A63">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>62</v>
@@ -9610,7 +9604,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="64" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A64">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>63</v>
@@ -9658,7 +9652,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="65" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A65">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>64</v>
@@ -9706,7 +9700,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="66" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A66">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>65</v>
@@ -9760,7 +9754,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="67" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A67">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>66</v>
@@ -9808,7 +9802,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="68" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A68">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>67</v>
@@ -9856,7 +9850,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="69" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A69">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>68</v>
@@ -9904,7 +9898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A70">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>69</v>
@@ -9952,7 +9946,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="71" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A71">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>70</v>
@@ -9997,7 +9991,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="72" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A72">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>71</v>
@@ -10051,7 +10045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:27" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>72</v>
@@ -10113,7 +10107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A74">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>73</v>
@@ -10161,7 +10155,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="75" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A75">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>74</v>
@@ -10721,7 +10715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A88">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>87</v>
@@ -10754,7 +10748,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="89" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A89">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>88</v>
@@ -10820,7 +10814,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="91" spans="1:27" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" ht="68" x14ac:dyDescent="0.2">
       <c r="A91">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>90</v>
@@ -10853,7 +10847,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="92" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A92">
         <f>ROW(Table3[[#This Row],[Id ]])-1</f>
         <v>91</v>

</xml_diff>

<commit_message>
Review icons and few powers. Fixed typos
</commit_message>
<xml_diff>
--- a/src/resources/horde_cards.xlsx
+++ b/src/resources/horde_cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsaban/git/perso/windwalkers-cardgame/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CFA064-34AD-D94C-A966-58EE87674F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A37CC9E-03B5-FF41-900D-4CBB1C56EA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="760" windowWidth="29120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="556">
   <si>
     <t>Id</t>
   </si>
@@ -953,9 +953,6 @@
   </si>
   <si>
     <t>Cassandre</t>
-  </si>
-  <si>
-    <t>assassin-maitre de l'univers</t>
   </si>
   <si>
     <t>Cassandre est une fille très colérique, mais qui peut révéler des ressources insoupçonnées.</t>
@@ -1333,9 +1330,6 @@
     <t>Selena, voyageuse opportuniste, retourne chaque situation à son avantage.</t>
   </si>
   <si>
-    <t>:discard:: Échangez votre position avec celle d'un joueur adjacent. Activez les bonus et/ou malus pour chacun.</t>
-  </si>
-  <si>
     <t>Selena.png</t>
   </si>
   <si>
@@ -1403,18 +1397,6 @@
     <t>:tap:: Annulez toutes vos actions, reculez et rejouez immédiatement.</t>
   </si>
   <si>
-    <t>:tap:: :discard: 1 :hordier: &lt;b&gt;FER/PACK/TRAÎNE&lt;/b&gt;. Remplacez-le par votre &lt;b&gt;Faucon&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>:tap:: Placez +1 :force-x: sur 3 :tuile: adjacentes.</t>
-  </si>
-  <si>
-    <t>:tap:: Lancez +1 :tous-mes-des: / :hordier: &lt;b&gt;FER&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>:tap:: Faites ±1 sur 1 :mes-des: / :hordier: &lt;b&gt;PACK&lt;/b&gt;.</t>
-  </si>
-  <si>
     <t>:tap:: Définissez une valeur et mettez tous :mes-des: sur cette valeur.</t>
   </si>
   <si>
@@ -1433,50 +1415,20 @@
     <t>:tap:: Équilibrez le :moral: des &lt;b&gt;Hordes&lt;/b&gt; adjacentes et le vôtre.</t>
   </si>
   <si>
-    <t>:tap:: Annulez le pouvoir d'un :hordier: dirigé contre votre &lt;b&gt;Horde&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>:discard:: Recrutez un :hordier: dans n'importe quel village.</t>
-  </si>
-  <si>
-    <t>:discard:: Forcer un joueur adjacent à changer un :hordier: avec un :hordier: aléatoire de la pioche.</t>
-  </si>
-  <si>
-    <t>:discard:: Lancez +1 :tous-mes-des: / :hordier: &lt;b&gt;PACK&lt;/b&gt;.</t>
-  </si>
-  <si>
     <t>:discard:: Lancez +1 :tous-mes-des: / :missing:</t>
   </si>
   <si>
     <t>:discard:: Faites ±1 sur :tous-mes-des: / :moral:</t>
-  </si>
-  <si>
-    <t>:tap:: Lancez +1 :mes-des: / :hordier: &lt;b&gt;oiseleur&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>Placez 1 :tous-mes-des: / :hordier: &lt;b&gt;Oiseleur&lt;/b&gt; puis :discard: &lt;b&gt;Hulan&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>:discard:: Choisissez un autre joueur. Il doit perdre -2 :moral: ou relancer le :mes-des: que vous désignez. S'il réussit son contre, regagnez +3 :moral:</t>
   </si>
   <si>
     <t>:tap:: Perdez -1 :moral: et lancez 1 :mes-des:.
 Si :mes-des: ≥ à :force-x:, ignorez tous :tous-des:</t>
   </si>
   <si>
-    <t>:tap:: Ignorez 1 :tous-des: / :terrain:</t>
-  </si>
-  <si>
     <t>:tap:: Faites ±1 sur la valeur de chacun de :mes-des:</t>
   </si>
   <si>
     <t>:tap:: Perdez -1 :moral:. Faites ±1 / :moral: restant sur :mes-des:</t>
-  </si>
-  <si>
-    <t>:tap:: Retirez une :tuile: grise du plateau. Si &lt;b&gt;Frank&lt;/b&gt; n'est pas dans votre équipe, perdez -1 :moral:</t>
-  </si>
-  <si>
-    <t>:tap:: Échangez 2 :tuile: grises et adjacentes à la vôtre. Si &lt;b&gt;Herbert&lt;/b&gt; n'est pas dans votre équipe, perdez -1 :moral:</t>
   </si>
   <si>
     <t>:tap:: Faites ±1 sur :mes-des: / :force-x:</t>
@@ -1498,9 +1450,6 @@
     <t>:tap:: Ignorez -1 :terrain: / :missing:</t>
   </si>
   <si>
-    <t>:tap:: Faites ±1 / &lt;b&gt;oiseleur&lt;/b&gt; sur 1 :mes-des:</t>
-  </si>
-  <si>
     <t>:tap:: Gagnez +1 :moral: / :missing:.
 Si vous :discard: &lt;b&gt;Zhalinka&lt;/b&gt;, :discard: &lt;b&gt;Oshora&lt;/b&gt; aussi puis activez son pouvoir</t>
   </si>
@@ -1508,55 +1457,24 @@
     <t>:tap:: :rest-all:. Perdez -1 :moral: / :rest:</t>
   </si>
   <si>
-    <t>:tap:: Lancez +1 :mes-des:. Si vous avez un autre &lt;b&gt;Torantor&lt;/b&gt;, faites ±1 sur 1 :mes-des:</t>
-  </si>
-  <si>
-    <t>:tap:: Lancez +1 :mes-des:. Si vous avez un autre &lt;b&gt;Torantor&lt;/b&gt;, gagnez +1 :moral:</t>
-  </si>
-  <si>
-    <t>:tap:: Si &lt;b&gt;Furevent&lt;/b&gt; :force-6:, :rest-all:</t>
-  </si>
-  <si>
     <t>:tap:: Placez 1 :mes-des:</t>
   </si>
   <si>
     <t>:tap:: Lancez +1 :mes-des: / :moral: sur :tuile:</t>
   </si>
   <si>
-    <t>:tap:: Si :tuile: = 3 :terrain:, gagnez +2 :moral:</t>
-  </si>
-  <si>
-    <t>:tap: :tuile: :force-x: ⮕ :force-1: Perdez -1 :moral:</t>
-  </si>
-  <si>
     <t>:tap:: Si :tuile: = 2 :terrain:, gagnez +2 :moral:</t>
   </si>
   <si>
-    <t>:tap:: Ignorez -1 :vent:</t>
-  </si>
-  <si>
-    <t>:discard:: Si vous avez un &lt;b&gt;oiseleur&lt;/b&gt;.
-Recrutez +1 :discard:</t>
-  </si>
-  <si>
     <t>:discard:: Recrutez 1 :discard:</t>
   </si>
   <si>
     <t>:tap:: Placez 1 :terrain:</t>
   </si>
   <si>
-    <t>:discard: :tuile: :force-x: ⮕ :force-2:</t>
-  </si>
-  <si>
     <t>:discard:: Ignorez -2 :tous-des:</t>
   </si>
   <si>
-    <t>:discard: :tuile: :force-x: ⮕ :force-3:</t>
-  </si>
-  <si>
-    <t>:discard: :tuile: :force-x: ⮕ :force-6:</t>
-  </si>
-  <si>
     <t>:tap:: Si vous rejoingnez une &lt;b&gt;Horde&lt;/b&gt;, ignorez tous les :tous-des:</t>
   </si>
   <si>
@@ -1564,9 +1482,6 @@
   </si>
   <si>
     <t>:tap:: Ignorez :vent: / :fatalite:</t>
-  </si>
-  <si>
-    <t>:tap:: Rajoutez +1 :fatalite: / :hordier: &lt;b&gt;géomaître&lt;/b&gt; sur une :tuile: adjacente ou sur la vôtre. Ces :fatalite: modifient définitivement la :tuile:</t>
   </si>
   <si>
     <t>:tap:: Prenez 1 :mes-des: à une &lt;b&gt;Horde&lt;/b&gt; devant vous. Si elle échoue son contre, perdez -1 :moral: Gagnez +1 :moral: sinon.</t>
@@ -1593,51 +1508,18 @@
 6 : Toutes les &lt;b&gt;Hordes&lt;/b&gt; gagnent +2 :moral:</t>
   </si>
   <si>
-    <t>:tap:: :tap: 1 autre :hordier: et gagnez +4 :moral:</t>
-  </si>
-  <si>
-    <t>:tap:: Échangez 1 :hordier: avec celui d’une autre &lt;b&gt;Horde&lt;/b&gt; sur votre :tuile:(sauf le &lt;b&gt;Traceur&lt;/b&gt;). Les deux &lt;b&gt;Hordes&lt;/b&gt; regagnent 1 :moral:</t>
-  </si>
-  <si>
     <t>:tap:: Déplacez une &lt;b&gt;Horde&lt;/b&gt; adjacente sur votre :tuile: Regagnez +3 :moral: si elle avance.</t>
   </si>
   <si>
-    <t>:tap:: Placez un de vos :hordier: &lt;b&gt;FER&lt;/b&gt; sur cette :hordier: Il compte comme &lt;b&gt;FER&lt;/b&gt; et &lt;b&gt;TRAÎNE&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>:tap:: Placez un de vos :hordier:  &lt;b&gt;PACK&lt;/b&gt; sur cette :hordier: Il compte comme &lt;b&gt;PACK&lt;/b&gt; et &lt;b&gt;TRAÎNE&lt;/b&gt;.</t>
-  </si>
-  <si>
     <t>:tap:: Ignorez TOUS :tous-des: Une fois utilisée, &lt;b&gt;Régitha&lt;/b&gt; ne peut être :discard:, remplacée ou :rest:</t>
   </si>
   <si>
-    <t>:tap: :discard: Tous les :fatalite: sont :terrain: et les :violet: sont :mes-des: :tuile: :force-x: ⮕ :force-1:</t>
-  </si>
-  <si>
     <t>:discard:: Gagnez +2 :moral: / :fatalite:</t>
   </si>
   <si>
     <t>:discard:: Ignorez :tous-des: &lt; à :force-x:</t>
   </si>
   <si>
-    <t>:discard:: Lancez +1 :violet: Si vous avez un autre :hordier: &lt;b&gt;Torantor&lt;/b&gt;, :rest: ce :hordier:</t>
-  </si>
-  <si>
-    <t>:discard:: Forcer un joueur à jouer un :hordier: que vous désignez s'il est sur votre :tuile:</t>
-  </si>
-  <si>
-    <t>:discard:: Annulez le pouvoir d'un :hordier:</t>
-  </si>
-  <si>
-    <t>:tap:: Placez +1 :force-x: Ignorez :tous-des: dont la valeur est &gt; à ce :force-x:</t>
-  </si>
-  <si>
-    <t>:tap:: Retirez -1 à :force-x: OU ajoutez +1 à :force-x: et gagnez +2 :moral:</t>
-  </si>
-  <si>
-    <t>:tap:: Si vous affrontez un &lt;b&gt;Choon&lt;/b&gt; :force-3:, gagnez +2 :moral:</t>
-  </si>
-  <si>
     <t>menuisier-croc</t>
   </si>
   <si>
@@ -1647,61 +1529,191 @@
     <t>:discard:: Placez 2 :tous-mes-des:</t>
   </si>
   <si>
+    <t>:tap:: Si :tuile: manquante autour de votre :tuile:, ignorez -3 :tous-des:</t>
+  </si>
+  <si>
+    <t>:discard:: Placez 1 :tous-mes-des: / :missing:</t>
+  </si>
+  <si>
+    <t>:tap:: Distribuez équitablement vos :fatalite: sur les :tuile: adjacentes, ces :fatalite: modifient définitivement la :tuile: puis :violet: = :mes-des:</t>
+  </si>
+  <si>
+    <t>:tap:: Lancez autant :mes-des: / Force :force-x:, ni plus, ni moins.</t>
+  </si>
+  <si>
+    <t>:discard:: Choisissez un autre Horde. Il doit perdre -2 :moral: ou relancer le :mes-des: que vous désignez. S'il réussit son contre, regagnez +3 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: Placez 1 :force-x: Ignorez :tous-des: dont la valeur est &gt; à ce :force-x:</t>
+  </si>
+  <si>
+    <t>:tap:: Ignorez -1 :tous-des: / :terrain:</t>
+  </si>
+  <si>
+    <t>:tap:: Lancez +1 :tous-mes-des: / :card: &lt;b&gt;FER&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:tap:: Faites ±1 sur 1 :mes-des: / :card: &lt;b&gt;PACK&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:discard:: Lancez +1 :tous-mes-des: / :card: &lt;b&gt;PACK&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:tap:: Retournez un :card: (n'importe lequel, n'importe où) si :rest: un :card: adverse, gagnez +3 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: :tuile: villages = :tuile: villes: Ignorez tous :tous-des: et vous recrutez tout type de :card: Si :rest-all: gagnez  +1 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: :discard: 1 :card: &lt;b&gt;TRAÎNE&lt;/b&gt;. 
+Placez :mes-des: / :missing: &lt;b&gt;TRAÎNE&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:tap:: Rajoutez +1 :fatalite: / :card: &lt;b&gt;géomaître&lt;/b&gt; sur une :tuile: adjacente ou sur la vôtre. Ces :fatalite: modifient définitivement la :tuile:</t>
+  </si>
+  <si>
+    <t>:tap:: :tap: 1 autre :card: et gagnez +4 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: Échangez 1 :card: avec celui d’une autre &lt;b&gt;Horde&lt;/b&gt; sur votre :tuile:(sauf le &lt;b&gt;Traceur&lt;/b&gt;). Les deux &lt;b&gt;Hordes&lt;/b&gt; regagnent 1 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: Annulez le pouvoir d'un :card: dirigé contre votre &lt;b&gt;Horde&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:discard:: Dévoilez +1 :card: / :tuile: village.</t>
+  </si>
+  <si>
+    <t>:tap:: Ignorez :terrain: / :card: &lt;b&gt;FEULEUR&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>:tap:: Lancez +1 :mes-des: / :card: &lt;b&gt;OISELEUR&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>Placez 1 :tous-mes-des: / :card: &lt;b&gt;OISELEUR&lt;/b&gt; puis :discard: &lt;b&gt;Hulan&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:tap:: Faites ±1 / &lt;b&gt;OISELEUR&lt;/b&gt; sur 1 :mes-des:</t>
+  </si>
+  <si>
+    <t>:discard:: Si vous avez 1 :card: &lt;b&gt;OISELEUR&lt;/b&gt;.
+Recrutez +1 :discard:</t>
+  </si>
+  <si>
+    <t>:discard:: Échangez votre position avec celle d'une Horde adjacent. Activez les bonus et/ou malus pour chacun.</t>
+  </si>
+  <si>
+    <t>:tap:: Utilisez un pouvoir :card: &lt;b&gt;TRAÎNE&lt;/b&gt; sans :discard:.
+:tap: ce :card:&lt;b&gt;TRAÎNE&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>:tap:: Lancez +1 :mes-des: Si vous avez 1 autre :card: &lt;b&gt;Torantor&lt;/b&gt;, :rest: cette :card:.</t>
+  </si>
+  <si>
+    <t>:tap:: Placez 1 de vos :card: &lt;b&gt;FER&lt;/b&gt; sur ce :card: Il compte comme &lt;b&gt;FER&lt;/b&gt; et &lt;b&gt;TRAÎNE&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:tap:: Placez 1 de vos :card:  &lt;b&gt;PACK&lt;/b&gt; sur ce :card: Il compte comme &lt;b&gt;PACK&lt;/b&gt; et &lt;b&gt;TRAÎNE&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:discard:: Recrutez 1 :card: dans n'importe quel village.</t>
+  </si>
+  <si>
+    <t>:discard:: Lancez +1 :violet:, :rest: 1 autre :card: &lt;b&gt;Torantor&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:discard:: Forcer une Horde adjacente à changer un :card: avec 1 :card: aléatoire de la pioche.</t>
+  </si>
+  <si>
+    <t>:discard:: Forcer une Horde à jouer 1 :card: que vous désignez s'il est sur votre :tuile:</t>
+  </si>
+  <si>
+    <t>:discard:: Annulez le pouvoir de 1 :card:</t>
+  </si>
+  <si>
+    <t>:tap:: Retirez une :tuile: grise du plateau. Si &lt;b&gt;FRANCK&lt;/b&gt; n'est pas dans votre équipe, perdez -1 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: Échangez 2 :tuile: grises et adjacentes à la vôtre. Si &lt;b&gt;HERBERT&lt;/b&gt; n'est pas dans votre équipe, perdez -1 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: :discard: 1 :card: &lt;b&gt;FER/PACK/TRAÎNE&lt;/b&gt;.
+Recrutez votre &lt;b&gt;Faucon&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:tap:: Retirez -1 à :force-x: 
+OU 
+ajoutez +1 à :force-x: et gagnez +2 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: Lancez +1 :mes-des:.
+Si vous avez un autre &lt;b&gt;TORANTOR&lt;/b&gt;, 
+Faites ±1 sur 1 :mes-des:</t>
+  </si>
+  <si>
+    <t>:tap:: Lancez +1 :mes-des:. 
+Si vous avez 1 autre &lt;b&gt;TORANTOR&lt;/b&gt;, 
+Gagnez +1 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: Placez 1 :force-x: sur 3 :tuile: adjacentes.</t>
+  </si>
+  <si>
+    <t>:tap:: Si :force-x: = &lt;b&gt;FUREVENT&lt;/b&gt; :force-6:, :rest-all:</t>
+  </si>
+  <si>
+    <t>:tap:: :force-x: ⮕ :force-1: Perdez -1 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: Ignorez -1 :epreuve:</t>
+  </si>
+  <si>
+    <t>recruteur-familier</t>
+  </si>
+  <si>
+    <t>:discard:: :force-x: ⮕ :force-2:</t>
+  </si>
+  <si>
+    <t>:discard:: :force-x: ⮕ :force-3:</t>
+  </si>
+  <si>
+    <t>:discard:: :force-x: ⮕ :force-6:</t>
+  </si>
+  <si>
     <t>:discard:: Gagnez +3 :moral:
-Si :discard: &lt;b&gt;Mère&lt;/b&gt; le même tour, regagnez tous vos :moral:</t>
+Si :discard: &lt;b&gt;Mère&lt;/b&gt; le même tour, regagnez tout :moral:</t>
   </si>
   <si>
     <t>:discard:: Gagnez +3 :moral:
-Si :discard: &lt;b&gt;Père&lt;/b&gt; le même tour, regagnez tous :moral:</t>
-  </si>
-  <si>
-    <t>:tap:: Si :tuile: manquante autour de votre :tuile:, ignorez -3 :tous-des:</t>
-  </si>
-  <si>
-    <t>:tap:: Utilisez un pouvoir :hordier: &lt;b&gt;TRAÎNE&lt;/b&gt; sans :discard:.
-:tap: cette :hordier:&lt;b&gt;TRAÎNE&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>:tap:: Retournez un :hordier: (n'importe lequel, n'importe où) si :rest: un :hordier: adverse, gagnez +3 :moral:</t>
-  </si>
-  <si>
-    <t>:tap:: Ignorez :terrain: / :hordier: &lt;b&gt;feuleur.se&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>:tap:: :discard: 1 :hordier: &lt;b&gt;TRACEUR/FER&lt;/b&gt;
-Recrutez un :hordier: &lt;b&gt;Calsan&lt;/b&gt; et :rest-all: &lt;b&gt;Calsans&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>:tap:: :discard: 1 :hordier: &lt;b&gt;TRAÎNE&lt;/b&gt;. 
-Placez :mes-des: / :missing: &lt;b&gt;TRAÎNE&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>:tap:: :discard: 1 :hordier: du &lt;b&gt;PACK&lt;/b&gt;. 
-Lancez :mes-des: / :missing: &lt;b&gt;PACK&lt;/b&gt;.</t>
-  </si>
-  <si>
-    <t>:discard:: Placez 1 :tous-mes-des: / :missing:</t>
-  </si>
-  <si>
-    <t>:discard:: Dévoilez +1 :force-x: / :tuile: adjacentes</t>
-  </si>
-  <si>
-    <t>:tap:: Distribuez équitablement vos :fatalite: sur les :tuile: adjacentes, ces :fatalite: modifient définitivement la :tuile: puis :violet: = :mes-des:</t>
-  </si>
-  <si>
-    <t>:tap:: Lancez autant :mes-des: / Force :force-x:, ni plus, ni moins.</t>
-  </si>
-  <si>
-    <t>:tap:: :tuile: villages = :tuile: villes: Ignorez tous :tous-des: et vous recrutez tout type de :hordier: Si :rest-all: gagnez  +1 :moral:</t>
-  </si>
-  <si>
-    <t>:tap:: Ignorez les :epreuve: et donnez &lt;b&gt;Cassandre&lt;/b&gt; à votre voisin de gauche. Cette &lt;b&gt;Horde&lt;/b&gt; :discard: &lt;b&gt;FER/TRACEUR&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>:discard:: Dévoilez +1 :hordier: / :tuile: village.</t>
-  </si>
-  <si>
-    <t>:tap:: Lancez +1 :mes-des: Si vous avez un autre :hordier: &lt;b&gt;Torantor&lt;/b&gt;, :rest: cette :hordier:.</t>
+Si :discard: &lt;b&gt;Père&lt;/b&gt; le même tour, regagnez tout :moral:</t>
+  </si>
+  <si>
+    <t>:discard:: Placez 1 :force-x: sur chaque :tuile: adjacente</t>
+  </si>
+  <si>
+    <t>:tap:: :discard: 1 :card: &lt;b&gt;PACK&lt;/b&gt;. 
+Lancez +1 :mes-des: / :missing: &lt;b&gt;PACK&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:tap:: :discard: 1 :card: &lt;b&gt;FER&lt;/b&gt;
+Recrutez 1 :card: &lt;b&gt;Calsan&lt;/b&gt; et :rest-all: &lt;b&gt;Calsans&lt;/b&gt;.</t>
+  </si>
+  <si>
+    <t>:tap:: Ignorez tous :epreuve: et donnez &lt;b&gt;Cassandre&lt;/b&gt; à votre voisin de gauche. 
+Cette &lt;b&gt;Horde&lt;/b&gt; :discard: &lt;b&gt;FER&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>assassin-princesse</t>
+  </si>
+  <si>
+    <t>:discard:: Tous les :fatalite: sont :terrain: et les :violet: sont :mes-des:
+:force-x: ⮕ :force-1:</t>
+  </si>
+  <si>
+    <t>:tap:: Si :force-x: = &lt;b&gt;CHOON&lt;/b&gt; :force-3:, gagnez +3 :moral:</t>
+  </si>
+  <si>
+    <t>:tap:: Si :tuile: = 3 :terrain:, gagnez +3 :moral:</t>
   </si>
 </sst>
 </file>
@@ -2080,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2190,7 +2202,7 @@
         <v>29</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="H2">
         <v>3</v>
@@ -2234,7 +2246,7 @@
         <v>35</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>532</v>
+        <v>504</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -2281,7 +2293,7 @@
         <v>39</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2319,7 +2331,7 @@
         <v>44</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -2363,7 +2375,7 @@
         <v>48</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>479</v>
+        <v>505</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -2407,7 +2419,7 @@
         <v>54</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -2451,7 +2463,7 @@
         <v>59</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="H8">
         <v>3</v>
@@ -2498,7 +2510,7 @@
         <v>64</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2539,7 +2551,7 @@
         <v>69</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>482</v>
+        <v>532</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2583,7 +2595,7 @@
         <v>72</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>483</v>
+        <v>533</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -2627,7 +2639,7 @@
         <v>76</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H12">
         <v>3</v>
@@ -2668,7 +2680,7 @@
         <v>80</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="H13">
         <v>2</v>
@@ -2715,7 +2727,7 @@
         <v>85</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -2765,7 +2777,7 @@
         <v>90</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>486</v>
+        <v>470</v>
       </c>
       <c r="H15">
         <v>3</v>
@@ -2806,10 +2818,10 @@
         <v>95</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="H16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" t="s">
         <v>96</v>
@@ -2856,7 +2868,7 @@
         <v>99</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>488</v>
+        <v>472</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -2906,7 +2918,7 @@
         <v>103</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>489</v>
+        <v>473</v>
       </c>
       <c r="H18">
         <v>2</v>
@@ -2956,7 +2968,7 @@
         <v>107</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>490</v>
+        <v>520</v>
       </c>
       <c r="H19">
         <v>3</v>
@@ -2997,7 +3009,7 @@
         <v>113</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -3027,7 +3039,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="64" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3047,7 +3059,7 @@
         <v>118</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>459</v>
+        <v>534</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -3071,7 +3083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3091,7 +3103,7 @@
         <v>121</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -3141,7 +3153,7 @@
         <v>125</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -3188,7 +3200,7 @@
         <v>130</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>534</v>
+        <v>554</v>
       </c>
       <c r="H24">
         <v>2</v>
@@ -3215,7 +3227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="64" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3235,7 +3247,7 @@
         <v>134</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>493</v>
+        <v>536</v>
       </c>
       <c r="H25">
         <v>3</v>
@@ -3265,7 +3277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="64" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3285,7 +3297,7 @@
         <v>134</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>494</v>
+        <v>537</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3335,7 +3347,7 @@
         <v>140</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>460</v>
+        <v>538</v>
       </c>
       <c r="H27">
         <v>3</v>
@@ -3362,7 +3374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3382,7 +3394,7 @@
         <v>144</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>495</v>
+        <v>539</v>
       </c>
       <c r="H28">
         <v>2</v>
@@ -3432,7 +3444,7 @@
         <v>148</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>496</v>
+        <v>476</v>
       </c>
       <c r="H29">
         <v>3</v>
@@ -3464,7 +3476,7 @@
         <v>150</v>
       </c>
       <c r="C30" t="s">
-        <v>535</v>
+        <v>496</v>
       </c>
       <c r="D30" t="s">
         <v>27</v>
@@ -3476,7 +3488,7 @@
         <v>151</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>461</v>
+        <v>506</v>
       </c>
       <c r="H30">
         <v>3</v>
@@ -3517,7 +3529,7 @@
         <v>155</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>497</v>
+        <v>477</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -3567,7 +3579,7 @@
         <v>159</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>498</v>
+        <v>555</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -3614,7 +3626,7 @@
         <v>163</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>499</v>
+        <v>540</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3664,7 +3676,7 @@
         <v>166</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3711,7 +3723,7 @@
         <v>170</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>536</v>
+        <v>497</v>
       </c>
       <c r="H35">
         <v>3</v>
@@ -3758,7 +3770,7 @@
         <v>173</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>501</v>
+        <v>541</v>
       </c>
       <c r="H36">
         <v>3</v>
@@ -3805,7 +3817,7 @@
         <v>178</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>462</v>
+        <v>507</v>
       </c>
       <c r="H37">
         <v>3</v>
@@ -3837,7 +3849,7 @@
         <v>180</v>
       </c>
       <c r="C38" t="s">
-        <v>181</v>
+        <v>542</v>
       </c>
       <c r="D38" t="s">
         <v>182</v>
@@ -3849,7 +3861,7 @@
         <v>184</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>502</v>
+        <v>521</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -3872,7 +3884,7 @@
         <v>186</v>
       </c>
       <c r="C39" t="s">
-        <v>181</v>
+        <v>542</v>
       </c>
       <c r="D39" t="s">
         <v>187</v>
@@ -3884,7 +3896,7 @@
         <v>188</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>503</v>
+        <v>479</v>
       </c>
       <c r="H39">
         <v>3</v>
@@ -3922,7 +3934,7 @@
         <v>192</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="H40">
         <v>3</v>
@@ -4004,7 +4016,7 @@
         <v>201</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>504</v>
+        <v>480</v>
       </c>
       <c r="H42">
         <v>3</v>
@@ -4045,7 +4057,7 @@
         <v>204</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>472</v>
+        <v>508</v>
       </c>
       <c r="H43">
         <v>3</v>
@@ -4086,7 +4098,7 @@
         <v>208</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>537</v>
+        <v>498</v>
       </c>
       <c r="H44">
         <v>2</v>
@@ -4107,7 +4119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4127,7 +4139,7 @@
         <v>212</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>505</v>
+        <v>543</v>
       </c>
       <c r="H45">
         <v>2</v>
@@ -4162,7 +4174,7 @@
         <v>215</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>506</v>
+        <v>481</v>
       </c>
       <c r="H46">
         <v>3</v>
@@ -4221,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4241,7 +4253,7 @@
         <v>223</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>507</v>
+        <v>544</v>
       </c>
       <c r="H48">
         <v>2</v>
@@ -4279,7 +4291,7 @@
         <v>227</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -4317,7 +4329,7 @@
         <v>230</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>547</v>
+        <v>500</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -4338,7 +4350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -4358,7 +4370,7 @@
         <v>233</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>508</v>
+        <v>545</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -4396,7 +4408,7 @@
         <v>237</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
       <c r="H52">
         <v>3</v>
@@ -4440,7 +4452,7 @@
         <v>241</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
       <c r="H53">
         <v>3</v>
@@ -4519,7 +4531,7 @@
         <v>249</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="H55">
         <v>3</v>
@@ -4557,7 +4569,7 @@
         <v>252</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>509</v>
+        <v>482</v>
       </c>
       <c r="H56">
         <v>2</v>
@@ -4575,7 +4587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="80" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4595,7 +4607,7 @@
         <v>256</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
       <c r="H57">
         <v>3</v>
@@ -4633,7 +4645,7 @@
         <v>259</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>549</v>
+        <v>501</v>
       </c>
       <c r="H58">
         <v>2</v>
@@ -4671,7 +4683,7 @@
         <v>263</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>540</v>
+        <v>499</v>
       </c>
       <c r="H59">
         <v>3</v>
@@ -4715,7 +4727,7 @@
         <v>266</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>542</v>
+        <v>509</v>
       </c>
       <c r="H60">
         <v>2</v>
@@ -4747,7 +4759,7 @@
         <v>269</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -4776,7 +4788,7 @@
         <v>272</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>551</v>
+        <v>510</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -4805,7 +4817,7 @@
         <v>275</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -4846,7 +4858,7 @@
         <v>279</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -4893,7 +4905,7 @@
         <v>283</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>550</v>
+        <v>502</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -4920,7 +4932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="80" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" ht="64" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4940,7 +4952,7 @@
         <v>287</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -4984,7 +4996,7 @@
         <v>290</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>545</v>
+        <v>511</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -5028,7 +5040,7 @@
         <v>294</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -5072,7 +5084,7 @@
         <v>299</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>543</v>
+        <v>517</v>
       </c>
       <c r="H69">
         <v>2</v>
@@ -5116,7 +5128,7 @@
         <v>303</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>511</v>
+        <v>484</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -5163,7 +5175,7 @@
         <v>307</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>475</v>
+        <v>518</v>
       </c>
       <c r="H71">
         <v>3</v>
@@ -5195,7 +5207,7 @@
         <v>310</v>
       </c>
       <c r="C72" t="s">
-        <v>311</v>
+        <v>552</v>
       </c>
       <c r="D72" t="s">
         <v>34</v>
@@ -5204,16 +5216,16 @@
         <v>53</v>
       </c>
       <c r="F72" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H72">
         <v>3</v>
       </c>
       <c r="I72" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J72" t="s">
         <v>254</v>
@@ -5224,10 +5236,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>313</v>
+      </c>
+      <c r="C73" t="s">
         <v>314</v>
-      </c>
-      <c r="C73" t="s">
-        <v>315</v>
       </c>
       <c r="D73" t="s">
         <v>27</v>
@@ -5236,7 +5248,7 @@
         <v>53</v>
       </c>
       <c r="F73" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>512</v>
@@ -5245,7 +5257,7 @@
         <v>2</v>
       </c>
       <c r="I73" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J73" t="s">
         <v>254</v>
@@ -5259,10 +5271,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>317</v>
+      </c>
+      <c r="C74" t="s">
         <v>318</v>
-      </c>
-      <c r="C74" t="s">
-        <v>319</v>
       </c>
       <c r="D74" t="s">
         <v>27</v>
@@ -5271,16 +5283,16 @@
         <v>53</v>
       </c>
       <c r="F74" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>513</v>
+        <v>485</v>
       </c>
       <c r="H74">
         <v>2</v>
       </c>
       <c r="I74" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J74" t="s">
         <v>254</v>
@@ -5291,10 +5303,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>321</v>
+      </c>
+      <c r="C75" t="s">
         <v>322</v>
-      </c>
-      <c r="C75" t="s">
-        <v>323</v>
       </c>
       <c r="D75" t="s">
         <v>34</v>
@@ -5303,16 +5315,16 @@
         <v>112</v>
       </c>
       <c r="F75" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>514</v>
+        <v>486</v>
       </c>
       <c r="H75">
         <v>2</v>
       </c>
       <c r="I75" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M75" t="s">
         <v>56</v>
@@ -5338,7 +5350,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C76" t="s">
         <v>89</v>
@@ -5350,16 +5362,16 @@
         <v>112</v>
       </c>
       <c r="F76" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="H76">
         <v>3</v>
       </c>
       <c r="I76" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M76" t="s">
         <v>46</v>
@@ -5382,10 +5394,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>328</v>
+      </c>
+      <c r="C77" t="s">
         <v>329</v>
-      </c>
-      <c r="C77" t="s">
-        <v>330</v>
       </c>
       <c r="D77" t="s">
         <v>34</v>
@@ -5394,16 +5406,16 @@
         <v>112</v>
       </c>
       <c r="F77" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>515</v>
+        <v>487</v>
       </c>
       <c r="H77">
         <v>2</v>
       </c>
       <c r="I77" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M77" t="s">
         <v>56</v>
@@ -5418,7 +5430,7 @@
         <v>1</v>
       </c>
       <c r="Z77" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="78" spans="1:26" ht="32" x14ac:dyDescent="0.2">
@@ -5426,10 +5438,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>333</v>
+      </c>
+      <c r="C78" t="s">
         <v>334</v>
-      </c>
-      <c r="C78" t="s">
-        <v>335</v>
       </c>
       <c r="D78" t="s">
         <v>27</v>
@@ -5438,16 +5450,16 @@
         <v>112</v>
       </c>
       <c r="F78" t="s">
+        <v>335</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78" t="s">
         <v>336</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="H78">
-        <v>1</v>
-      </c>
-      <c r="I78" t="s">
-        <v>337</v>
       </c>
       <c r="M78" t="s">
         <v>175</v>
@@ -5467,7 +5479,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C79" t="s">
         <v>133</v>
@@ -5479,16 +5491,16 @@
         <v>112</v>
       </c>
       <c r="F79" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>554</v>
+        <v>524</v>
       </c>
       <c r="H79">
         <v>3</v>
       </c>
       <c r="I79" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M79" t="s">
         <v>92</v>
@@ -5514,7 +5526,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C80" t="s">
         <v>63</v>
@@ -5526,16 +5538,16 @@
         <v>112</v>
       </c>
       <c r="F80" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>517</v>
+        <v>489</v>
       </c>
       <c r="H80">
         <v>3</v>
       </c>
       <c r="I80" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J80" t="s">
         <v>254</v>
@@ -5561,7 +5573,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C81" t="s">
         <v>154</v>
@@ -5573,16 +5585,16 @@
         <v>112</v>
       </c>
       <c r="F81" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>518</v>
+        <v>490</v>
       </c>
       <c r="H81">
         <v>2</v>
       </c>
       <c r="I81" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M81" t="s">
         <v>109</v>
@@ -5602,10 +5614,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>346</v>
+      </c>
+      <c r="C82" t="s">
         <v>347</v>
-      </c>
-      <c r="C82" t="s">
-        <v>348</v>
       </c>
       <c r="D82" t="s">
         <v>27</v>
@@ -5614,16 +5626,16 @@
         <v>112</v>
       </c>
       <c r="F82" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>519</v>
+        <v>491</v>
       </c>
       <c r="H82">
         <v>2</v>
       </c>
       <c r="I82" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="83" spans="1:26" ht="48" x14ac:dyDescent="0.2">
@@ -5631,28 +5643,28 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>350</v>
+      </c>
+      <c r="C83" t="s">
         <v>351</v>
       </c>
-      <c r="C83" t="s">
-        <v>352</v>
-      </c>
       <c r="D83" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E83" t="s">
         <v>112</v>
       </c>
       <c r="F83" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="H83">
         <v>3</v>
       </c>
       <c r="I83" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="84" spans="1:26" ht="48" x14ac:dyDescent="0.2">
@@ -5660,10 +5672,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
+        <v>354</v>
+      </c>
+      <c r="C84" t="s">
         <v>355</v>
-      </c>
-      <c r="C84" t="s">
-        <v>356</v>
       </c>
       <c r="D84" t="s">
         <v>34</v>
@@ -5672,16 +5684,16 @@
         <v>112</v>
       </c>
       <c r="F84" t="s">
+        <v>356</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
         <v>357</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="H84">
-        <v>1</v>
-      </c>
-      <c r="I84" t="s">
-        <v>358</v>
       </c>
       <c r="J84" t="s">
         <v>254</v>
@@ -5692,7 +5704,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C85" t="s">
         <v>94</v>
@@ -5704,16 +5716,16 @@
         <v>112</v>
       </c>
       <c r="F85" t="s">
+        <v>359</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85" t="s">
         <v>360</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="H85">
-        <v>1</v>
-      </c>
-      <c r="I85" t="s">
-        <v>361</v>
       </c>
       <c r="J85" t="s">
         <v>254</v>
@@ -5724,7 +5736,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C86" t="s">
         <v>52</v>
@@ -5736,16 +5748,16 @@
         <v>112</v>
       </c>
       <c r="F86" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="H86">
         <v>2</v>
       </c>
       <c r="I86" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J86" t="s">
         <v>254</v>
@@ -5756,10 +5768,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
+        <v>364</v>
+      </c>
+      <c r="C87" t="s">
         <v>365</v>
-      </c>
-      <c r="C87" t="s">
-        <v>366</v>
       </c>
       <c r="D87" t="s">
         <v>34</v>
@@ -5768,16 +5780,16 @@
         <v>112</v>
       </c>
       <c r="F87" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="H87">
         <v>3</v>
       </c>
       <c r="I87" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J87" t="s">
         <v>254</v>
@@ -5788,7 +5800,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C88" t="s">
         <v>75</v>
@@ -5800,16 +5812,16 @@
         <v>112</v>
       </c>
       <c r="F88" t="s">
+        <v>369</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88" t="s">
         <v>370</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88" t="s">
-        <v>371</v>
       </c>
       <c r="J88" t="s">
         <v>254</v>
@@ -5820,10 +5832,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
+        <v>371</v>
+      </c>
+      <c r="C89" t="s">
         <v>372</v>
-      </c>
-      <c r="C89" t="s">
-        <v>373</v>
       </c>
       <c r="D89" t="s">
         <v>34</v>
@@ -5832,16 +5844,16 @@
         <v>112</v>
       </c>
       <c r="F89" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>522</v>
+        <v>492</v>
       </c>
       <c r="H89">
         <v>2</v>
       </c>
       <c r="I89" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J89" t="s">
         <v>254</v>
@@ -5852,7 +5864,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C90" t="s">
         <v>211</v>
@@ -5864,16 +5876,16 @@
         <v>183</v>
       </c>
       <c r="F90" t="s">
+        <v>376</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90" t="s">
         <v>377</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="H90">
-        <v>1</v>
-      </c>
-      <c r="I90" t="s">
-        <v>378</v>
       </c>
       <c r="V90">
         <v>1</v>
@@ -5884,7 +5896,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C91" t="s">
         <v>211</v>
@@ -5896,16 +5908,16 @@
         <v>183</v>
       </c>
       <c r="F91" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="H91">
         <v>1</v>
       </c>
       <c r="I91" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="V91">
         <v>1</v>
@@ -5916,7 +5928,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C92" t="s">
         <v>236</v>
@@ -5928,16 +5940,16 @@
         <v>183</v>
       </c>
       <c r="F92" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>525</v>
+        <v>493</v>
       </c>
       <c r="H92">
         <v>2</v>
       </c>
       <c r="I92" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="T92">
         <v>1</v>
@@ -5951,10 +5963,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
+        <v>383</v>
+      </c>
+      <c r="C93" t="s">
         <v>384</v>
-      </c>
-      <c r="C93" t="s">
-        <v>385</v>
       </c>
       <c r="D93" t="s">
         <v>27</v>
@@ -5963,16 +5975,16 @@
         <v>183</v>
       </c>
       <c r="F93" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>526</v>
+        <v>553</v>
       </c>
       <c r="H93">
         <v>3</v>
       </c>
       <c r="I93" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="M93" t="s">
         <v>56</v>
@@ -5989,10 +6001,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>387</v>
+      </c>
+      <c r="C94" t="s">
         <v>388</v>
-      </c>
-      <c r="C94" t="s">
-        <v>389</v>
       </c>
       <c r="D94" t="s">
         <v>34</v>
@@ -6001,16 +6013,16 @@
         <v>183</v>
       </c>
       <c r="F94" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>527</v>
+        <v>494</v>
       </c>
       <c r="H94">
         <v>2</v>
       </c>
       <c r="I94" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S94">
         <v>1</v>
@@ -6022,15 +6034,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:26" ht="48" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>391</v>
+      </c>
+      <c r="C95" t="s">
         <v>392</v>
-      </c>
-      <c r="C95" t="s">
-        <v>393</v>
       </c>
       <c r="D95" t="s">
         <v>34</v>
@@ -6039,16 +6051,16 @@
         <v>183</v>
       </c>
       <c r="F95" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>470</v>
+        <v>527</v>
       </c>
       <c r="H95">
         <v>3</v>
       </c>
       <c r="I95" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="R95">
         <v>1</v>
@@ -6059,10 +6071,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C96" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D96" t="s">
         <v>34</v>
@@ -6071,16 +6083,16 @@
         <v>183</v>
       </c>
       <c r="F96" t="s">
+        <v>396</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96" t="s">
         <v>397</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="H96">
-        <v>1</v>
-      </c>
-      <c r="I96" t="s">
-        <v>398</v>
       </c>
       <c r="R96">
         <v>1</v>
@@ -6091,7 +6103,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C97" t="s">
         <v>181</v>
@@ -6103,16 +6115,16 @@
         <v>183</v>
       </c>
       <c r="F97" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>528</v>
+        <v>495</v>
       </c>
       <c r="H97">
         <v>2</v>
       </c>
       <c r="I97" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q97">
         <v>1</v>
@@ -6129,10 +6141,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
+        <v>401</v>
+      </c>
+      <c r="C98" t="s">
         <v>402</v>
-      </c>
-      <c r="C98" t="s">
-        <v>403</v>
       </c>
       <c r="D98" t="s">
         <v>34</v>
@@ -6141,17 +6153,17 @@
         <v>183</v>
       </c>
       <c r="F98" t="s">
+        <v>403</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98" t="s">
         <v>404</v>
       </c>
-      <c r="G98" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98" t="s">
-        <v>405</v>
-      </c>
       <c r="S98">
         <v>1</v>
       </c>
@@ -6159,12 +6171,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:24" ht="64" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:24" ht="32" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C99" t="s">
         <v>200</v>
@@ -6176,16 +6188,16 @@
         <v>183</v>
       </c>
       <c r="F99" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H99">
         <v>2</v>
       </c>
       <c r="I99" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M99" t="s">
         <v>92</v>
@@ -6202,7 +6214,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C100" t="s">
         <v>236</v>
@@ -6214,16 +6226,16 @@
         <v>183</v>
       </c>
       <c r="F100" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>477</v>
+        <v>503</v>
       </c>
       <c r="H100">
         <v>2</v>
       </c>
       <c r="I100" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J100" t="s">
         <v>254</v>
@@ -6234,7 +6246,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C101" t="s">
         <v>222</v>
@@ -6246,16 +6258,16 @@
         <v>183</v>
       </c>
       <c r="F101" t="s">
+        <v>412</v>
+      </c>
+      <c r="G101" s="3" t="s">
         <v>413</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>414</v>
       </c>
       <c r="H101">
         <v>3</v>
       </c>
       <c r="I101" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="102" spans="1:24" ht="144" x14ac:dyDescent="0.2">
@@ -6263,10 +6275,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
+        <v>415</v>
+      </c>
+      <c r="C102" t="s">
         <v>416</v>
-      </c>
-      <c r="C102" t="s">
-        <v>417</v>
       </c>
       <c r="D102" t="s">
         <v>34</v>
@@ -6275,16 +6287,16 @@
         <v>183</v>
       </c>
       <c r="F102" t="s">
+        <v>417</v>
+      </c>
+      <c r="G102" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="G102" s="3" t="s">
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102" t="s">
         <v>419</v>
-      </c>
-      <c r="H102">
-        <v>1</v>
-      </c>
-      <c r="I102" t="s">
-        <v>420</v>
       </c>
       <c r="J102" t="s">
         <v>254</v>
@@ -6295,7 +6307,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C103" t="s">
         <v>181</v>
@@ -6307,16 +6319,16 @@
         <v>183</v>
       </c>
       <c r="F103" t="s">
+        <v>421</v>
+      </c>
+      <c r="G103" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="G103" s="3" t="s">
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103" t="s">
         <v>423</v>
-      </c>
-      <c r="H103">
-        <v>1</v>
-      </c>
-      <c r="I103" t="s">
-        <v>424</v>
       </c>
       <c r="V103">
         <v>1</v>
@@ -6327,7 +6339,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C104" t="s">
         <v>195</v>
@@ -6339,16 +6351,16 @@
         <v>183</v>
       </c>
       <c r="F104" t="s">
+        <v>425</v>
+      </c>
+      <c r="G104" s="3" t="s">
         <v>426</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>427</v>
       </c>
       <c r="H104">
         <v>3</v>
       </c>
       <c r="I104" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="S104">
         <v>1</v>
@@ -6362,7 +6374,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C105" t="s">
         <v>222</v>
@@ -6374,16 +6386,16 @@
         <v>183</v>
       </c>
       <c r="F105" t="s">
+        <v>429</v>
+      </c>
+      <c r="G105" s="3" t="s">
         <v>430</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>431</v>
       </c>
       <c r="H105">
         <v>3</v>
       </c>
       <c r="I105" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J105" t="s">
         <v>254</v>
@@ -6394,10 +6406,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
+        <v>432</v>
+      </c>
+      <c r="C106" t="s">
         <v>433</v>
-      </c>
-      <c r="C106" t="s">
-        <v>434</v>
       </c>
       <c r="D106" t="s">
         <v>34</v>
@@ -6406,30 +6418,30 @@
         <v>183</v>
       </c>
       <c r="F106" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>436</v>
+        <v>522</v>
       </c>
       <c r="H106">
         <v>2</v>
       </c>
       <c r="I106" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="J106" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="107" spans="1:24" ht="80" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:24" ht="64" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C107" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D107" t="s">
         <v>27</v>
@@ -6438,30 +6450,30 @@
         <v>183</v>
       </c>
       <c r="F107" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>471</v>
+        <v>529</v>
       </c>
       <c r="H107">
         <v>1</v>
       </c>
       <c r="I107" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J107" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="108" spans="1:24" ht="64" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:24" ht="48" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C108" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D108" t="s">
         <v>27</v>
@@ -6470,7 +6482,7 @@
         <v>183</v>
       </c>
       <c r="F108" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>530</v>
@@ -6479,7 +6491,7 @@
         <v>1</v>
       </c>
       <c r="I108" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J108" t="s">
         <v>254</v>
@@ -6490,10 +6502,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C109" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D109" t="s">
         <v>34</v>
@@ -6502,7 +6514,7 @@
         <v>183</v>
       </c>
       <c r="F109" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>531</v>
@@ -6511,7 +6523,7 @@
         <v>1</v>
       </c>
       <c r="I109" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J109" t="s">
         <v>254</v>
@@ -6522,25 +6534,25 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C110" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E110" t="s">
         <v>183</v>
       </c>
       <c r="F110" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H110">
         <v>2</v>
       </c>
       <c r="I110" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J110" t="s">
         <v>254</v>

</xml_diff>